<commit_message>
Changes of 29th march 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" tabRatio="614"/>
+    <workbookView tabRatio="614" windowHeight="9660" windowWidth="19815" xWindow="390" yWindow="510"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Sno</t>
   </si>
@@ -194,6 +194,15 @@
   </si>
   <si>
     <t>{"attempt":{ "newReadyTime": "02/28/2022 10:26", "attemptCount": 1}}</t>
+  </si>
+  <si>
+    <t>320018165046</t>
+  </si>
+  <si>
+    <t>320018165080</t>
+  </si>
+  <si>
+    <t>320018165090</t>
   </si>
 </sst>
 </file>
@@ -259,35 +268,38 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -301,10 +313,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -462,7 +474,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -471,13 +483,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -487,7 +499,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -496,7 +508,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,7 +517,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -515,12 +527,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -551,7 +563,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -570,7 +582,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -582,29 +594,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="28.140625" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" customWidth="1"/>
-    <col min="11" max="11" width="104.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="104.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25">
+    <row ht="26.25" r="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -647,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -668,7 +680,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -688,7 +700,7 @@
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="6"/>
@@ -711,10 +723,10 @@
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="2"/>
@@ -736,10 +748,10 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>57</v>
       </c>
       <c r="E6" s="2"/>
@@ -761,10 +773,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="2"/>
@@ -881,10 +893,10 @@
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="2"/>
@@ -904,10 +916,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="2"/>
@@ -927,10 +939,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="2"/>
@@ -950,10 +962,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="2"/>
@@ -973,10 +985,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="2"/>
@@ -1017,7 +1029,7 @@
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="5"/>
@@ -1038,7 +1050,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" t="s">
+      <c r="C20" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="5"/>
@@ -1059,7 +1071,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="5"/>
@@ -1075,7 +1087,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="26.25">
+    <row ht="26.25" r="22" spans="1:11">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1096,8 +1108,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="26.25">
-      <c r="A23" s="1">
+    <row ht="26.25" r="23" spans="1:11">
+      <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
@@ -1129,7 +1141,7 @@
       <c r="K24" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of cheetah processing
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="188">
   <si>
     <t>Sno</t>
   </si>
@@ -203,6 +203,381 @@
   </si>
   <si>
     <t>320018165090</t>
+  </si>
+  <si>
+    <t>320018165127</t>
+  </si>
+  <si>
+    <t>320018165138</t>
+  </si>
+  <si>
+    <t>320018165160</t>
+  </si>
+  <si>
+    <t>320018165182</t>
+  </si>
+  <si>
+    <t>320018165220</t>
+  </si>
+  <si>
+    <t>320018165241</t>
+  </si>
+  <si>
+    <t>320018165274</t>
+  </si>
+  <si>
+    <t>320018165296</t>
+  </si>
+  <si>
+    <t>320018165322</t>
+  </si>
+  <si>
+    <t>320018165344</t>
+  </si>
+  <si>
+    <t>320018165388</t>
+  </si>
+  <si>
+    <t>320018165403</t>
+  </si>
+  <si>
+    <t>320018165436</t>
+  </si>
+  <si>
+    <t>320018165458</t>
+  </si>
+  <si>
+    <t>320018165480</t>
+  </si>
+  <si>
+    <t>320018165506</t>
+  </si>
+  <si>
+    <t>320018165540</t>
+  </si>
+  <si>
+    <t>320018165561</t>
+  </si>
+  <si>
+    <t>320018165594</t>
+  </si>
+  <si>
+    <t>320018165610</t>
+  </si>
+  <si>
+    <t>320018165642</t>
+  </si>
+  <si>
+    <t>320018165653</t>
+  </si>
+  <si>
+    <t>320018165664</t>
+  </si>
+  <si>
+    <t>320018165697</t>
+  </si>
+  <si>
+    <t>320018165712</t>
+  </si>
+  <si>
+    <t>320018165756</t>
+  </si>
+  <si>
+    <t>320018167016</t>
+  </si>
+  <si>
+    <t>320018167027</t>
+  </si>
+  <si>
+    <t>320018175850</t>
+  </si>
+  <si>
+    <t>320018175860</t>
+  </si>
+  <si>
+    <t>320018175893</t>
+  </si>
+  <si>
+    <t>320018175919</t>
+  </si>
+  <si>
+    <t>320018175952</t>
+  </si>
+  <si>
+    <t>320018175996</t>
+  </si>
+  <si>
+    <t>320018176010</t>
+  </si>
+  <si>
+    <t>320018176043</t>
+  </si>
+  <si>
+    <t>320018176065</t>
+  </si>
+  <si>
+    <t>320018176113</t>
+  </si>
+  <si>
+    <t>320018176135</t>
+  </si>
+  <si>
+    <t>320018176179</t>
+  </si>
+  <si>
+    <t>320018176190</t>
+  </si>
+  <si>
+    <t>320018176227</t>
+  </si>
+  <si>
+    <t>320018176249</t>
+  </si>
+  <si>
+    <t>320018176271</t>
+  </si>
+  <si>
+    <t>320018176293</t>
+  </si>
+  <si>
+    <t>320018176341</t>
+  </si>
+  <si>
+    <t>320018176374</t>
+  </si>
+  <si>
+    <t>320018176400</t>
+  </si>
+  <si>
+    <t>320018176422</t>
+  </si>
+  <si>
+    <t>320018176455</t>
+  </si>
+  <si>
+    <t>320018176488</t>
+  </si>
+  <si>
+    <t>320018176499</t>
+  </si>
+  <si>
+    <t>320018176503</t>
+  </si>
+  <si>
+    <t>320018176536</t>
+  </si>
+  <si>
+    <t>320018176558</t>
+  </si>
+  <si>
+    <t>320018176591</t>
+  </si>
+  <si>
+    <t>320018176617</t>
+  </si>
+  <si>
+    <t>320018176694</t>
+  </si>
+  <si>
+    <t>320018176720</t>
+  </si>
+  <si>
+    <t>320018176742</t>
+  </si>
+  <si>
+    <t>320018176786</t>
+  </si>
+  <si>
+    <t>320018176801</t>
+  </si>
+  <si>
+    <t>320018176834</t>
+  </si>
+  <si>
+    <t>320018177050</t>
+  </si>
+  <si>
+    <t>320018177061</t>
+  </si>
+  <si>
+    <t>320018177094</t>
+  </si>
+  <si>
+    <t>320018177278</t>
+  </si>
+  <si>
+    <t>320018177315</t>
+  </si>
+  <si>
+    <t>320018177337</t>
+  </si>
+  <si>
+    <t>320018177360</t>
+  </si>
+  <si>
+    <t>320018177381</t>
+  </si>
+  <si>
+    <t>320018177418</t>
+  </si>
+  <si>
+    <t>320018177430</t>
+  </si>
+  <si>
+    <t>320018177473</t>
+  </si>
+  <si>
+    <t>320018177500</t>
+  </si>
+  <si>
+    <t>320018177532</t>
+  </si>
+  <si>
+    <t>320018177554</t>
+  </si>
+  <si>
+    <t>320018177587</t>
+  </si>
+  <si>
+    <t>320018177602</t>
+  </si>
+  <si>
+    <t>320018177679</t>
+  </si>
+  <si>
+    <t>320018177690</t>
+  </si>
+  <si>
+    <t>320018179189</t>
+  </si>
+  <si>
+    <t>320018179190</t>
+  </si>
+  <si>
+    <t>320018179226</t>
+  </si>
+  <si>
+    <t>320018179454</t>
+  </si>
+  <si>
+    <t>320018179498</t>
+  </si>
+  <si>
+    <t>320018179513</t>
+  </si>
+  <si>
+    <t>320018179546</t>
+  </si>
+  <si>
+    <t>320018179568</t>
+  </si>
+  <si>
+    <t>320018179590</t>
+  </si>
+  <si>
+    <t>320018179616</t>
+  </si>
+  <si>
+    <t>320018179650</t>
+  </si>
+  <si>
+    <t>320018179671</t>
+  </si>
+  <si>
+    <t>320018179708</t>
+  </si>
+  <si>
+    <t>320018179720</t>
+  </si>
+  <si>
+    <t>320018179752</t>
+  </si>
+  <si>
+    <t>320018179774</t>
+  </si>
+  <si>
+    <t>320018179811</t>
+  </si>
+  <si>
+    <t>320018179833</t>
+  </si>
+  <si>
+    <t>320018179866</t>
+  </si>
+  <si>
+    <t>320018179888</t>
+  </si>
+  <si>
+    <t>320018179914</t>
+  </si>
+  <si>
+    <t>320018179947</t>
+  </si>
+  <si>
+    <t>320018179958</t>
+  </si>
+  <si>
+    <t>320018179991</t>
+  </si>
+  <si>
+    <t>320018180002</t>
+  </si>
+  <si>
+    <t>320018180035</t>
+  </si>
+  <si>
+    <t>320018180057</t>
+  </si>
+  <si>
+    <t>320018180090</t>
+  </si>
+  <si>
+    <t>320018180127</t>
+  </si>
+  <si>
+    <t>320018180150</t>
+  </si>
+  <si>
+    <t>320018180171</t>
+  </si>
+  <si>
+    <t>320018180208</t>
+  </si>
+  <si>
+    <t>320018180220</t>
+  </si>
+  <si>
+    <t>320018180263</t>
+  </si>
+  <si>
+    <t>320018180285</t>
+  </si>
+  <si>
+    <t>320018180311</t>
+  </si>
+  <si>
+    <t>320018180333</t>
+  </si>
+  <si>
+    <t>320018180366</t>
+  </si>
+  <si>
+    <t>320018180388</t>
+  </si>
+  <si>
+    <t>320018180425</t>
+  </si>
+  <si>
+    <t>320018180447</t>
+  </si>
+  <si>
+    <t>320018180480</t>
+  </si>
+  <si>
+    <t>320018180506</t>
+  </si>
+  <si>
+    <t>320018180539</t>
   </si>
 </sst>
 </file>
@@ -659,7 +1034,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -680,7 +1055,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -700,8 +1075,8 @@
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>55</v>
+      <c r="C4" t="s">
+        <v>169</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -723,11 +1098,11 @@
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>56</v>
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
+        <v>170</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -748,11 +1123,11 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>57</v>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -773,11 +1148,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>58</v>
+      <c r="C7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" t="s">
+        <v>172</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -796,7 +1171,9 @@
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
+      <c r="C8" t="s">
+        <v>173</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
@@ -815,7 +1192,9 @@
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
+      <c r="C9" t="s">
+        <v>174</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
@@ -834,7 +1213,9 @@
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="6"/>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
@@ -853,7 +1234,9 @@
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
+      <c r="C11" t="s">
+        <v>176</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
@@ -872,7 +1255,9 @@
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
@@ -893,11 +1278,11 @@
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>45</v>
+      <c r="C13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" t="s">
+        <v>178</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -916,11 +1301,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>46</v>
+      <c r="C14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" t="s">
+        <v>179</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -939,11 +1324,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>47</v>
+      <c r="C15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" t="s">
+        <v>180</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -962,11 +1347,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>48</v>
+      <c r="C16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" t="s">
+        <v>181</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -985,11 +1370,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>49</v>
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" t="s">
+        <v>182</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1008,7 +1393,9 @@
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
+      <c r="C18" t="s">
+        <v>183</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
       <c r="F18" s="7" t="s">
@@ -1029,8 +1416,8 @@
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>50</v>
+      <c r="C19" t="s">
+        <v>184</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
@@ -1050,8 +1437,8 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="6" t="s">
-        <v>51</v>
+      <c r="C20" t="s">
+        <v>185</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
@@ -1071,8 +1458,8 @@
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="6" t="s">
-        <v>52</v>
+      <c r="C21" t="s">
+        <v>186</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
@@ -1094,7 +1481,9 @@
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" t="s">
+        <v>187</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">

</xml_diff>

<commit_message>
Changes of 31st March 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="229">
   <si>
     <t>Sno</t>
   </si>
@@ -578,6 +578,129 @@
   </si>
   <si>
     <t>320018180539</t>
+  </si>
+  <si>
+    <t>320018191411</t>
+  </si>
+  <si>
+    <t>320018191422</t>
+  </si>
+  <si>
+    <t>320018191455</t>
+  </si>
+  <si>
+    <t>320018191477</t>
+  </si>
+  <si>
+    <t>320018191514</t>
+  </si>
+  <si>
+    <t>320018191536</t>
+  </si>
+  <si>
+    <t>320018191569</t>
+  </si>
+  <si>
+    <t>320018191580</t>
+  </si>
+  <si>
+    <t>320018191617</t>
+  </si>
+  <si>
+    <t>320018191639</t>
+  </si>
+  <si>
+    <t>320018191672</t>
+  </si>
+  <si>
+    <t>320018191694</t>
+  </si>
+  <si>
+    <t>320018191720</t>
+  </si>
+  <si>
+    <t>320018191742</t>
+  </si>
+  <si>
+    <t>320018191775</t>
+  </si>
+  <si>
+    <t>320018191797</t>
+  </si>
+  <si>
+    <t>320018191834</t>
+  </si>
+  <si>
+    <t>320018191856</t>
+  </si>
+  <si>
+    <t>320018191889</t>
+  </si>
+  <si>
+    <t>320018191904</t>
+  </si>
+  <si>
+    <t>320018191948</t>
+  </si>
+  <si>
+    <t>320018191959</t>
+  </si>
+  <si>
+    <t>320018191981</t>
+  </si>
+  <si>
+    <t>320018192006</t>
+  </si>
+  <si>
+    <t>320018192040</t>
+  </si>
+  <si>
+    <t>320018192061</t>
+  </si>
+  <si>
+    <t>320018192094</t>
+  </si>
+  <si>
+    <t>320018192131</t>
+  </si>
+  <si>
+    <t>320018192164</t>
+  </si>
+  <si>
+    <t>320018192186</t>
+  </si>
+  <si>
+    <t>320018192223</t>
+  </si>
+  <si>
+    <t>320018192245</t>
+  </si>
+  <si>
+    <t>320018192278</t>
+  </si>
+  <si>
+    <t>320018192290</t>
+  </si>
+  <si>
+    <t>320018192326</t>
+  </si>
+  <si>
+    <t>320018192348</t>
+  </si>
+  <si>
+    <t>320018192381</t>
+  </si>
+  <si>
+    <t>320018192407</t>
+  </si>
+  <si>
+    <t>320018192430</t>
+  </si>
+  <si>
+    <t>320018192451</t>
+  </si>
+  <si>
+    <t>320018192484</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>208</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -1055,7 +1178,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -1076,7 +1199,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -1099,10 +1222,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1124,10 +1247,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1149,10 +1272,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1172,7 +1295,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -1193,7 +1316,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -1214,7 +1337,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>216</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -1235,7 +1358,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>217</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -1256,7 +1379,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -1279,10 +1402,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1302,10 +1425,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>220</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>220</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1325,10 +1448,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1348,10 +1471,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1371,10 +1494,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>223</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>223</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1394,7 +1517,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
@@ -1417,7 +1540,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>184</v>
+        <v>225</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
@@ -1438,7 +1561,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>185</v>
+        <v>226</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
@@ -1459,7 +1582,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
@@ -1482,7 +1605,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>187</v>
+        <v>228</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 1st april 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="265">
   <si>
     <t>Sno</t>
   </si>
@@ -701,6 +701,114 @@
   </si>
   <si>
     <t>320018192484</t>
+  </si>
+  <si>
+    <t>320018207701</t>
+  </si>
+  <si>
+    <t>320018207712</t>
+  </si>
+  <si>
+    <t>320018207745</t>
+  </si>
+  <si>
+    <t>320018207804</t>
+  </si>
+  <si>
+    <t>320018207815</t>
+  </si>
+  <si>
+    <t>320018207848</t>
+  </si>
+  <si>
+    <t>320018207860</t>
+  </si>
+  <si>
+    <t>320018207907</t>
+  </si>
+  <si>
+    <t>320018207929</t>
+  </si>
+  <si>
+    <t>320018207951</t>
+  </si>
+  <si>
+    <t>320018207973</t>
+  </si>
+  <si>
+    <t>320018208009</t>
+  </si>
+  <si>
+    <t>320018208020</t>
+  </si>
+  <si>
+    <t>320018208064</t>
+  </si>
+  <si>
+    <t>320018208086</t>
+  </si>
+  <si>
+    <t>320018208097</t>
+  </si>
+  <si>
+    <t>320018208101</t>
+  </si>
+  <si>
+    <t>320018208134</t>
+  </si>
+  <si>
+    <t>320018208156</t>
+  </si>
+  <si>
+    <t>320018208190</t>
+  </si>
+  <si>
+    <t>320018208215</t>
+  </si>
+  <si>
+    <t>320018208248</t>
+  </si>
+  <si>
+    <t>320018208260</t>
+  </si>
+  <si>
+    <t>320018208292</t>
+  </si>
+  <si>
+    <t>320018208318</t>
+  </si>
+  <si>
+    <t>320018208351</t>
+  </si>
+  <si>
+    <t>320018208373</t>
+  </si>
+  <si>
+    <t>320018208400</t>
+  </si>
+  <si>
+    <t>320018208421</t>
+  </si>
+  <si>
+    <t>320018208454</t>
+  </si>
+  <si>
+    <t>320018208476</t>
+  </si>
+  <si>
+    <t>320018208513</t>
+  </si>
+  <si>
+    <t>320018208535</t>
+  </si>
+  <si>
+    <t>320018208568</t>
+  </si>
+  <si>
+    <t>320018208580</t>
+  </si>
+  <si>
+    <t>320018208616</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>244</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -1178,7 +1286,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -1199,7 +1307,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -1222,10 +1330,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="D5" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1247,10 +1355,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="D6" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1272,10 +1380,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>213</v>
+        <v>249</v>
       </c>
       <c r="D7" t="s">
-        <v>213</v>
+        <v>249</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1295,7 +1403,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -1316,7 +1424,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>251</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -1337,7 +1445,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>252</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -1358,7 +1466,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -1379,7 +1487,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -1402,10 +1510,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="D13" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1425,10 +1533,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c r="D14" t="s">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1448,10 +1556,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c r="D15" t="s">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1471,10 +1579,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="D16" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1494,10 +1602,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="D17" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1517,7 +1625,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
@@ -1540,7 +1648,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
@@ -1561,7 +1669,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
@@ -1582,7 +1690,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>227</v>
+        <v>263</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
@@ -1605,7 +1713,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 5th April
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="266">
   <si>
     <t>Sno</t>
   </si>
@@ -809,6 +809,9 @@
   </si>
   <si>
     <t>320018208616</t>
+  </si>
+  <si>
+    <t>320018248263</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1268,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>

</xml_diff>

<commit_message>
Changes of 6th April 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="328">
   <si>
     <t>Sno</t>
   </si>
@@ -812,6 +812,192 @@
   </si>
   <si>
     <t>320018248263</t>
+  </si>
+  <si>
+    <t>320018248274</t>
+  </si>
+  <si>
+    <t>320018248300</t>
+  </si>
+  <si>
+    <t>320018248322</t>
+  </si>
+  <si>
+    <t>320018248366</t>
+  </si>
+  <si>
+    <t>320018248388</t>
+  </si>
+  <si>
+    <t>320018248414</t>
+  </si>
+  <si>
+    <t>320018248436</t>
+  </si>
+  <si>
+    <t>320018248469</t>
+  </si>
+  <si>
+    <t>320018248480</t>
+  </si>
+  <si>
+    <t>320018248528</t>
+  </si>
+  <si>
+    <t>320018248540</t>
+  </si>
+  <si>
+    <t>320018248572</t>
+  </si>
+  <si>
+    <t>320018248594</t>
+  </si>
+  <si>
+    <t>320018248620</t>
+  </si>
+  <si>
+    <t>320018248642</t>
+  </si>
+  <si>
+    <t>320018248686</t>
+  </si>
+  <si>
+    <t>320018248723</t>
+  </si>
+  <si>
+    <t>320018248756</t>
+  </si>
+  <si>
+    <t>320018248778</t>
+  </si>
+  <si>
+    <t>320018248804</t>
+  </si>
+  <si>
+    <t>320018251605</t>
+  </si>
+  <si>
+    <t>320018251616</t>
+  </si>
+  <si>
+    <t>320018251649</t>
+  </si>
+  <si>
+    <t>320018251660</t>
+  </si>
+  <si>
+    <t>320018251708</t>
+  </si>
+  <si>
+    <t>320018251720</t>
+  </si>
+  <si>
+    <t>320018251752</t>
+  </si>
+  <si>
+    <t>320018251774</t>
+  </si>
+  <si>
+    <t>320018251800</t>
+  </si>
+  <si>
+    <t>320018251822</t>
+  </si>
+  <si>
+    <t>320018251866</t>
+  </si>
+  <si>
+    <t>320018251888</t>
+  </si>
+  <si>
+    <t>320018251914</t>
+  </si>
+  <si>
+    <t>320018251936</t>
+  </si>
+  <si>
+    <t>320018251969</t>
+  </si>
+  <si>
+    <t>320018251980</t>
+  </si>
+  <si>
+    <t>320018252027</t>
+  </si>
+  <si>
+    <t>320018252049</t>
+  </si>
+  <si>
+    <t>320018252071</t>
+  </si>
+  <si>
+    <t>320018252093</t>
+  </si>
+  <si>
+    <t>320018252120</t>
+  </si>
+  <si>
+    <t>320018252380</t>
+  </si>
+  <si>
+    <t>320018252391</t>
+  </si>
+  <si>
+    <t>320018252428</t>
+  </si>
+  <si>
+    <t>320018252461</t>
+  </si>
+  <si>
+    <t>320018252520</t>
+  </si>
+  <si>
+    <t>320018252564</t>
+  </si>
+  <si>
+    <t>320018252612</t>
+  </si>
+  <si>
+    <t>320018252656</t>
+  </si>
+  <si>
+    <t>320018252689</t>
+  </si>
+  <si>
+    <t>320018252704</t>
+  </si>
+  <si>
+    <t>320018252748</t>
+  </si>
+  <si>
+    <t>320018252760</t>
+  </si>
+  <si>
+    <t>320018252807</t>
+  </si>
+  <si>
+    <t>320018252829</t>
+  </si>
+  <si>
+    <t>320018252873</t>
+  </si>
+  <si>
+    <t>320018252910</t>
+  </si>
+  <si>
+    <t>320018252976</t>
+  </si>
+  <si>
+    <t>320018253012</t>
+  </si>
+  <si>
+    <t>320018253240</t>
+  </si>
+  <si>
+    <t>320018253284</t>
+  </si>
+  <si>
+    <t>320018253354</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1454,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>307</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -1289,7 +1475,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>308</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -1310,7 +1496,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>309</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -1333,10 +1519,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>247</v>
+        <v>310</v>
       </c>
       <c r="D5" t="s">
-        <v>247</v>
+        <v>310</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1358,10 +1544,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>248</v>
+        <v>311</v>
       </c>
       <c r="D6" t="s">
-        <v>248</v>
+        <v>311</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1383,10 +1569,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>249</v>
+        <v>312</v>
       </c>
       <c r="D7" t="s">
-        <v>249</v>
+        <v>312</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1406,7 +1592,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>250</v>
+        <v>313</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -1427,7 +1613,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>251</v>
+        <v>314</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -1448,7 +1634,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>315</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -1469,7 +1655,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>253</v>
+        <v>316</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -1490,7 +1676,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>317</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -1513,10 +1699,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>255</v>
+        <v>318</v>
       </c>
       <c r="D13" t="s">
-        <v>255</v>
+        <v>318</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1536,10 +1722,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>256</v>
+        <v>319</v>
       </c>
       <c r="D14" t="s">
-        <v>256</v>
+        <v>319</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1559,10 +1745,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>257</v>
+        <v>320</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>320</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1582,10 +1768,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>258</v>
+        <v>321</v>
       </c>
       <c r="D16" t="s">
-        <v>258</v>
+        <v>321</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1605,10 +1791,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>259</v>
+        <v>322</v>
       </c>
       <c r="D17" t="s">
-        <v>259</v>
+        <v>322</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1628,7 +1814,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>260</v>
+        <v>323</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
@@ -1651,7 +1837,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>261</v>
+        <v>324</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
@@ -1672,7 +1858,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>262</v>
+        <v>325</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
@@ -1693,7 +1879,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>263</v>
+        <v>326</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
@@ -1716,7 +1902,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>264</v>
+        <v>327</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 27Th April 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="532">
   <si>
     <t>Sno</t>
   </si>
@@ -998,6 +998,618 @@
   </si>
   <si>
     <t>320018253354</t>
+  </si>
+  <si>
+    <t>320018256721</t>
+  </si>
+  <si>
+    <t>320018256732</t>
+  </si>
+  <si>
+    <t>320018256765</t>
+  </si>
+  <si>
+    <t>320018256787</t>
+  </si>
+  <si>
+    <t>320018256824</t>
+  </si>
+  <si>
+    <t>320018256846</t>
+  </si>
+  <si>
+    <t>320018256879</t>
+  </si>
+  <si>
+    <t>320018256890</t>
+  </si>
+  <si>
+    <t>320018256927</t>
+  </si>
+  <si>
+    <t>320018256949</t>
+  </si>
+  <si>
+    <t>320018256982</t>
+  </si>
+  <si>
+    <t>320018257007</t>
+  </si>
+  <si>
+    <t>320018257030</t>
+  </si>
+  <si>
+    <t>320018257051</t>
+  </si>
+  <si>
+    <t>320018257084</t>
+  </si>
+  <si>
+    <t>320018257100</t>
+  </si>
+  <si>
+    <t>320018257143</t>
+  </si>
+  <si>
+    <t>320018257165</t>
+  </si>
+  <si>
+    <t>320018257198</t>
+  </si>
+  <si>
+    <t>320018257213</t>
+  </si>
+  <si>
+    <t>320018257246</t>
+  </si>
+  <si>
+    <t>320018261878</t>
+  </si>
+  <si>
+    <t>320018261889</t>
+  </si>
+  <si>
+    <t>320018261915</t>
+  </si>
+  <si>
+    <t>320018261937</t>
+  </si>
+  <si>
+    <t>320018261970</t>
+  </si>
+  <si>
+    <t>320018261992</t>
+  </si>
+  <si>
+    <t>320018262028</t>
+  </si>
+  <si>
+    <t>320018262040</t>
+  </si>
+  <si>
+    <t>320018262072</t>
+  </si>
+  <si>
+    <t>320018262094</t>
+  </si>
+  <si>
+    <t>320018262131</t>
+  </si>
+  <si>
+    <t>320018262153</t>
+  </si>
+  <si>
+    <t>320018262186</t>
+  </si>
+  <si>
+    <t>320018262201</t>
+  </si>
+  <si>
+    <t>320018262234</t>
+  </si>
+  <si>
+    <t>320018262256</t>
+  </si>
+  <si>
+    <t>320018262290</t>
+  </si>
+  <si>
+    <t>320018262315</t>
+  </si>
+  <si>
+    <t>320018262348</t>
+  </si>
+  <si>
+    <t>320018262360</t>
+  </si>
+  <si>
+    <t>320018262392</t>
+  </si>
+  <si>
+    <t>320018274889</t>
+  </si>
+  <si>
+    <t>320018274890</t>
+  </si>
+  <si>
+    <t>320018274926</t>
+  </si>
+  <si>
+    <t>320018274959</t>
+  </si>
+  <si>
+    <t>320018275197</t>
+  </si>
+  <si>
+    <t>320018275212</t>
+  </si>
+  <si>
+    <t>320018275245</t>
+  </si>
+  <si>
+    <t>320018275267</t>
+  </si>
+  <si>
+    <t>320018275290</t>
+  </si>
+  <si>
+    <t>320018275315</t>
+  </si>
+  <si>
+    <t>320018275360</t>
+  </si>
+  <si>
+    <t>320018275381</t>
+  </si>
+  <si>
+    <t>320018275418</t>
+  </si>
+  <si>
+    <t>320018275430</t>
+  </si>
+  <si>
+    <t>320018275473</t>
+  </si>
+  <si>
+    <t>320018275495</t>
+  </si>
+  <si>
+    <t>320018275543</t>
+  </si>
+  <si>
+    <t>320018275565</t>
+  </si>
+  <si>
+    <t>320018275598</t>
+  </si>
+  <si>
+    <t>320018275613</t>
+  </si>
+  <si>
+    <t>320018275657</t>
+  </si>
+  <si>
+    <t>320018278840</t>
+  </si>
+  <si>
+    <t>320018278851</t>
+  </si>
+  <si>
+    <t>320018278884</t>
+  </si>
+  <si>
+    <t>320018278900</t>
+  </si>
+  <si>
+    <t>320018278954</t>
+  </si>
+  <si>
+    <t>320018278976</t>
+  </si>
+  <si>
+    <t>320018279001</t>
+  </si>
+  <si>
+    <t>320018279023</t>
+  </si>
+  <si>
+    <t>320018279056</t>
+  </si>
+  <si>
+    <t>320018279078</t>
+  </si>
+  <si>
+    <t>320018279115</t>
+  </si>
+  <si>
+    <t>320018279137</t>
+  </si>
+  <si>
+    <t>320018279160</t>
+  </si>
+  <si>
+    <t>320018279192</t>
+  </si>
+  <si>
+    <t>320018279229</t>
+  </si>
+  <si>
+    <t>320018279240</t>
+  </si>
+  <si>
+    <t>320018279284</t>
+  </si>
+  <si>
+    <t>320018279300</t>
+  </si>
+  <si>
+    <t>320018279332</t>
+  </si>
+  <si>
+    <t>320018279354</t>
+  </si>
+  <si>
+    <t>320018279387</t>
+  </si>
+  <si>
+    <t>320018289344</t>
+  </si>
+  <si>
+    <t>320018289355</t>
+  </si>
+  <si>
+    <t>320018289388</t>
+  </si>
+  <si>
+    <t>320018289403</t>
+  </si>
+  <si>
+    <t>320018289447</t>
+  </si>
+  <si>
+    <t>320018289469</t>
+  </si>
+  <si>
+    <t>320018289491</t>
+  </si>
+  <si>
+    <t>320018289517</t>
+  </si>
+  <si>
+    <t>320018289540</t>
+  </si>
+  <si>
+    <t>320018289561</t>
+  </si>
+  <si>
+    <t>320018289609</t>
+  </si>
+  <si>
+    <t>320018289620</t>
+  </si>
+  <si>
+    <t>320018289653</t>
+  </si>
+  <si>
+    <t>320018289675</t>
+  </si>
+  <si>
+    <t>320018289701</t>
+  </si>
+  <si>
+    <t>320018289723</t>
+  </si>
+  <si>
+    <t>320018289767</t>
+  </si>
+  <si>
+    <t>320018289789</t>
+  </si>
+  <si>
+    <t>320018289815</t>
+  </si>
+  <si>
+    <t>320018289837</t>
+  </si>
+  <si>
+    <t>320018289860</t>
+  </si>
+  <si>
+    <t>320018309442</t>
+  </si>
+  <si>
+    <t>320018309453</t>
+  </si>
+  <si>
+    <t>320018309486</t>
+  </si>
+  <si>
+    <t>320018309501</t>
+  </si>
+  <si>
+    <t>320018309545</t>
+  </si>
+  <si>
+    <t>320018309567</t>
+  </si>
+  <si>
+    <t>320018309590</t>
+  </si>
+  <si>
+    <t>320018309615</t>
+  </si>
+  <si>
+    <t>320018309648</t>
+  </si>
+  <si>
+    <t>320018309660</t>
+  </si>
+  <si>
+    <t>320018309707</t>
+  </si>
+  <si>
+    <t>320018309729</t>
+  </si>
+  <si>
+    <t>320018309751</t>
+  </si>
+  <si>
+    <t>320018309773</t>
+  </si>
+  <si>
+    <t>320018309800</t>
+  </si>
+  <si>
+    <t>320018309821</t>
+  </si>
+  <si>
+    <t>320018321535</t>
+  </si>
+  <si>
+    <t>320018321546</t>
+  </si>
+  <si>
+    <t>320018321579</t>
+  </si>
+  <si>
+    <t>320018321590</t>
+  </si>
+  <si>
+    <t>320018321638</t>
+  </si>
+  <si>
+    <t>320018321650</t>
+  </si>
+  <si>
+    <t>320018321682</t>
+  </si>
+  <si>
+    <t>320018321708</t>
+  </si>
+  <si>
+    <t>320018321730</t>
+  </si>
+  <si>
+    <t>320018321752</t>
+  </si>
+  <si>
+    <t>320018321796</t>
+  </si>
+  <si>
+    <t>320018321811</t>
+  </si>
+  <si>
+    <t>320018321844</t>
+  </si>
+  <si>
+    <t>320018321866</t>
+  </si>
+  <si>
+    <t>320018321899</t>
+  </si>
+  <si>
+    <t>320018321914</t>
+  </si>
+  <si>
+    <t>320018321958</t>
+  </si>
+  <si>
+    <t>320018321970</t>
+  </si>
+  <si>
+    <t>320018322005</t>
+  </si>
+  <si>
+    <t>320018322027</t>
+  </si>
+  <si>
+    <t>320018322050</t>
+  </si>
+  <si>
+    <t>320018330996</t>
+  </si>
+  <si>
+    <t>320018331000</t>
+  </si>
+  <si>
+    <t>320018331032</t>
+  </si>
+  <si>
+    <t>320018331054</t>
+  </si>
+  <si>
+    <t>320018331098</t>
+  </si>
+  <si>
+    <t>320018331113</t>
+  </si>
+  <si>
+    <t>320018331146</t>
+  </si>
+  <si>
+    <t>320018331168</t>
+  </si>
+  <si>
+    <t>320018331190</t>
+  </si>
+  <si>
+    <t>320018331216</t>
+  </si>
+  <si>
+    <t>320018331250</t>
+  </si>
+  <si>
+    <t>320018331271</t>
+  </si>
+  <si>
+    <t>320018331308</t>
+  </si>
+  <si>
+    <t>320018331320</t>
+  </si>
+  <si>
+    <t>320018331352</t>
+  </si>
+  <si>
+    <t>320018331374</t>
+  </si>
+  <si>
+    <t>320018331411</t>
+  </si>
+  <si>
+    <t>320018331433</t>
+  </si>
+  <si>
+    <t>320018331466</t>
+  </si>
+  <si>
+    <t>320018331488</t>
+  </si>
+  <si>
+    <t>320018331514</t>
+  </si>
+  <si>
+    <t>320018363678</t>
+  </si>
+  <si>
+    <t>320018363689</t>
+  </si>
+  <si>
+    <t>320018363715</t>
+  </si>
+  <si>
+    <t>320018363737</t>
+  </si>
+  <si>
+    <t>320018363770</t>
+  </si>
+  <si>
+    <t>320018363792</t>
+  </si>
+  <si>
+    <t>320018363829</t>
+  </si>
+  <si>
+    <t>320018363840</t>
+  </si>
+  <si>
+    <t>320018363873</t>
+  </si>
+  <si>
+    <t>320018363895</t>
+  </si>
+  <si>
+    <t>320018363932</t>
+  </si>
+  <si>
+    <t>320018363954</t>
+  </si>
+  <si>
+    <t>320018363987</t>
+  </si>
+  <si>
+    <t>320018364001</t>
+  </si>
+  <si>
+    <t>320018364034</t>
+  </si>
+  <si>
+    <t>320018364056</t>
+  </si>
+  <si>
+    <t>320018364090</t>
+  </si>
+  <si>
+    <t>320018364115</t>
+  </si>
+  <si>
+    <t>320018364148</t>
+  </si>
+  <si>
+    <t>320018364160</t>
+  </si>
+  <si>
+    <t>320018364192</t>
+  </si>
+  <si>
+    <t>320018387090</t>
+  </si>
+  <si>
+    <t>320018387105</t>
+  </si>
+  <si>
+    <t>320018387138</t>
+  </si>
+  <si>
+    <t>320018387150</t>
+  </si>
+  <si>
+    <t>320018387193</t>
+  </si>
+  <si>
+    <t>320018387219</t>
+  </si>
+  <si>
+    <t>320018387241</t>
+  </si>
+  <si>
+    <t>320018387263</t>
+  </si>
+  <si>
+    <t>320018387296</t>
+  </si>
+  <si>
+    <t>320018387311</t>
+  </si>
+  <si>
+    <t>320018387355</t>
+  </si>
+  <si>
+    <t>320018387377</t>
+  </si>
+  <si>
+    <t>320018387403</t>
+  </si>
+  <si>
+    <t>320018387425</t>
+  </si>
+  <si>
+    <t>320018387458</t>
+  </si>
+  <si>
+    <t>320018387470</t>
+  </si>
+  <si>
+    <t>320018387517</t>
+  </si>
+  <si>
+    <t>320018387539</t>
+  </si>
+  <si>
+    <t>320018387561</t>
+  </si>
+  <si>
+    <t>320018387583</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +2002,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -1454,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>512</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -1475,7 +2087,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>308</v>
+        <v>513</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -1496,7 +2108,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>309</v>
+        <v>514</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -1519,10 +2131,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>515</v>
       </c>
       <c r="D5" t="s">
-        <v>310</v>
+        <v>515</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1544,10 +2156,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>311</v>
+        <v>516</v>
       </c>
       <c r="D6" t="s">
-        <v>311</v>
+        <v>516</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1569,10 +2181,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>312</v>
+        <v>517</v>
       </c>
       <c r="D7" t="s">
-        <v>312</v>
+        <v>517</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1592,7 +2204,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>313</v>
+        <v>518</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -1613,7 +2225,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>314</v>
+        <v>519</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -1634,7 +2246,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>315</v>
+        <v>520</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -1655,7 +2267,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>316</v>
+        <v>521</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -1676,7 +2288,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>317</v>
+        <v>522</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -1699,10 +2311,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>318</v>
+        <v>523</v>
       </c>
       <c r="D13" t="s">
-        <v>318</v>
+        <v>523</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1722,10 +2334,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>319</v>
+        <v>524</v>
       </c>
       <c r="D14" t="s">
-        <v>319</v>
+        <v>524</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1745,10 +2357,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>320</v>
+        <v>525</v>
       </c>
       <c r="D15" t="s">
-        <v>320</v>
+        <v>525</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1768,10 +2380,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>321</v>
+        <v>526</v>
       </c>
       <c r="D16" t="s">
-        <v>321</v>
+        <v>526</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1791,10 +2403,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>322</v>
+        <v>527</v>
       </c>
       <c r="D17" t="s">
-        <v>322</v>
+        <v>527</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1814,7 +2426,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>323</v>
+        <v>528</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
@@ -1837,7 +2449,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>324</v>
+        <v>529</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
@@ -1858,7 +2470,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>325</v>
+        <v>530</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
@@ -1879,7 +2491,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>531</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
@@ -1902,7 +2514,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>327</v>
+        <v>511</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
final change of 27th April 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="556">
   <si>
     <t>Sno</t>
   </si>
@@ -1610,6 +1610,78 @@
   </si>
   <si>
     <t>320018387583</t>
+  </si>
+  <si>
+    <t>320018398352</t>
+  </si>
+  <si>
+    <t>320018404671</t>
+  </si>
+  <si>
+    <t>320018407085</t>
+  </si>
+  <si>
+    <t>320018407199</t>
+  </si>
+  <si>
+    <t>320018407203</t>
+  </si>
+  <si>
+    <t>320018407236</t>
+  </si>
+  <si>
+    <t>320018407269</t>
+  </si>
+  <si>
+    <t>320018407306</t>
+  </si>
+  <si>
+    <t>320018407328</t>
+  </si>
+  <si>
+    <t>320018407361</t>
+  </si>
+  <si>
+    <t>320018407394</t>
+  </si>
+  <si>
+    <t>320018407420</t>
+  </si>
+  <si>
+    <t>320018407442</t>
+  </si>
+  <si>
+    <t>320018407486</t>
+  </si>
+  <si>
+    <t>320018407501</t>
+  </si>
+  <si>
+    <t>320018407740</t>
+  </si>
+  <si>
+    <t>320018407773</t>
+  </si>
+  <si>
+    <t>320018407810</t>
+  </si>
+  <si>
+    <t>320018407832</t>
+  </si>
+  <si>
+    <t>320018407876</t>
+  </si>
+  <si>
+    <t>320018407898</t>
+  </si>
+  <si>
+    <t>320018407924</t>
+  </si>
+  <si>
+    <t>320018407946</t>
+  </si>
+  <si>
+    <t>320018407979</t>
   </si>
 </sst>
 </file>
@@ -2002,7 +2074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -2066,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>512</v>
+        <v>535</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -2087,7 +2159,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>513</v>
+        <v>536</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -2108,7 +2180,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>514</v>
+        <v>537</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -2131,10 +2203,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>515</v>
+        <v>538</v>
       </c>
       <c r="D5" t="s">
-        <v>515</v>
+        <v>538</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2156,10 +2228,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>516</v>
+        <v>539</v>
       </c>
       <c r="D6" t="s">
-        <v>516</v>
+        <v>539</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -2181,10 +2253,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>517</v>
+        <v>540</v>
       </c>
       <c r="D7" t="s">
-        <v>517</v>
+        <v>540</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -2204,7 +2276,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -2225,7 +2297,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>519</v>
+        <v>542</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -2246,7 +2318,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>520</v>
+        <v>543</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -2267,7 +2339,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>521</v>
+        <v>544</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -2288,7 +2360,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>522</v>
+        <v>545</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -2311,10 +2383,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>523</v>
+        <v>546</v>
       </c>
       <c r="D13" t="s">
-        <v>523</v>
+        <v>546</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2334,10 +2406,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>524</v>
+        <v>547</v>
       </c>
       <c r="D14" t="s">
-        <v>524</v>
+        <v>547</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2357,10 +2429,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>525</v>
+        <v>548</v>
       </c>
       <c r="D15" t="s">
-        <v>525</v>
+        <v>548</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2380,10 +2452,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>526</v>
+        <v>549</v>
       </c>
       <c r="D16" t="s">
-        <v>526</v>
+        <v>549</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2403,10 +2475,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="D17" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2426,7 +2498,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>528</v>
+        <v>551</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
@@ -2449,7 +2521,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>529</v>
+        <v>552</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
@@ -2470,7 +2542,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>530</v>
+        <v>553</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
@@ -2491,7 +2563,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>531</v>
+        <v>554</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
@@ -2514,7 +2586,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>511</v>
+        <v>555</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Latest final changes of 29th April 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView tabRatio="614" windowHeight="9660" windowWidth="19815" xWindow="390" yWindow="510"/>
+    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" tabRatio="614"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
   <si>
     <t>Sno</t>
   </si>
@@ -154,133 +154,100 @@
     <t>{"attempt":{ "newReadyTime": "02/28/2022 10:26", "attemptCount": 1}}</t>
   </si>
   <si>
-    <t>320018414433</t>
-  </si>
-  <si>
-    <t>320018414444</t>
-  </si>
-  <si>
-    <t>320018414477</t>
-  </si>
-  <si>
-    <t>320018414499</t>
-  </si>
-  <si>
-    <t>320018414536</t>
-  </si>
-  <si>
-    <t>320018414558</t>
-  </si>
-  <si>
-    <t>320018414580</t>
-  </si>
-  <si>
-    <t>320018414617</t>
-  </si>
-  <si>
-    <t>320018414640</t>
-  </si>
-  <si>
-    <t>320018414661</t>
-  </si>
-  <si>
-    <t>320018414709</t>
-  </si>
-  <si>
-    <t>320018414720</t>
-  </si>
-  <si>
-    <t>320018414753</t>
-  </si>
-  <si>
-    <t>320018414775</t>
-  </si>
-  <si>
-    <t>320018414801</t>
-  </si>
-  <si>
-    <t>320018414823</t>
-  </si>
-  <si>
-    <t>320018414867</t>
-  </si>
-  <si>
-    <t>320018414889</t>
-  </si>
-  <si>
-    <t>320018414915</t>
-  </si>
-  <si>
-    <t>320018414937</t>
-  </si>
-  <si>
-    <t>320018414960</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>320018417432</t>
-  </si>
-  <si>
-    <t>320018417443</t>
-  </si>
-  <si>
-    <t>320018417476</t>
-  </si>
-  <si>
-    <t>320018417498</t>
-  </si>
-  <si>
-    <t>320018417535</t>
-  </si>
-  <si>
-    <t>320018417557</t>
-  </si>
-  <si>
-    <t>320018417580</t>
-  </si>
-  <si>
-    <t>320018417605</t>
-  </si>
-  <si>
-    <t>320018417649</t>
-  </si>
-  <si>
-    <t>320018417660</t>
-  </si>
-  <si>
-    <t>320018417708</t>
-  </si>
-  <si>
-    <t>320018417720</t>
-  </si>
-  <si>
-    <t>320018417752</t>
-  </si>
-  <si>
-    <t>320018417774</t>
-  </si>
-  <si>
-    <t>320018417800</t>
-  </si>
-  <si>
-    <t>320018417822</t>
-  </si>
-  <si>
-    <t>320018417866</t>
-  </si>
-  <si>
-    <t>320018417888</t>
-  </si>
-  <si>
-    <t>320018417914</t>
-  </si>
-  <si>
-    <t>320018417936</t>
-  </si>
-  <si>
-    <t>320018417969</t>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>PickedUp</t>
+  </si>
+  <si>
+    <t>PuStatusUpdate</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>DelStatusUpdate</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>packageDetailChange</t>
+  </si>
+  <si>
+    <t>addPackage</t>
+  </si>
+  <si>
+    <t>PickupException(PAT)</t>
+  </si>
+  <si>
+    <t>320018428083</t>
+  </si>
+  <si>
+    <t>320018428131</t>
+  </si>
+  <si>
+    <t>320018427514</t>
+  </si>
+  <si>
+    <t>320018427525</t>
+  </si>
+  <si>
+    <t>320018427558</t>
+  </si>
+  <si>
+    <t>320018427570</t>
+  </si>
+  <si>
+    <t>320018427617</t>
+  </si>
+  <si>
+    <t>320018427639</t>
+  </si>
+  <si>
+    <t>320018427661</t>
+  </si>
+  <si>
+    <t>320018427683</t>
+  </si>
+  <si>
+    <t>320018427710</t>
+  </si>
+  <si>
+    <t>320018427731</t>
+  </si>
+  <si>
+    <t>320018427775</t>
+  </si>
+  <si>
+    <t>320018427797</t>
+  </si>
+  <si>
+    <t>320018427823</t>
+  </si>
+  <si>
+    <t>320018427845</t>
+  </si>
+  <si>
+    <t>320018427878</t>
+  </si>
+  <si>
+    <t>320018427890</t>
+  </si>
+  <si>
+    <t>320018427937</t>
+  </si>
+  <si>
+    <t>320018427959</t>
+  </si>
+  <si>
+    <t>320018427981</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -290,7 +257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -304,6 +271,12 @@
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -321,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -344,40 +317,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -391,10 +408,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -552,7 +569,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -561,13 +578,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -577,7 +594,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -586,7 +603,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -595,7 +612,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -605,12 +622,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -641,7 +658,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -660,7 +677,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -672,30 +689,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="104.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="104.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="26.25" r="1" spans="1:12">
+    <row r="1" spans="1:30" ht="39">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -729,21 +758,75 @@
       <c r="K1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="L1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="5"/>
+      <c r="C2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="12"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
@@ -753,18 +836,47 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+    </row>
+    <row r="3" spans="1:30" ht="14.25" customHeight="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="12"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
@@ -774,18 +886,39 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="13"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
@@ -797,19 +930,48 @@
       <c r="K4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="L4" s="11"/>
+      <c r="M4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>71</v>
+      <c r="C5" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -822,19 +984,48 @@
       <c r="K5" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="L5" s="11"/>
+      <c r="M5" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>72</v>
+      <c r="C6" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -849,17 +1040,50 @@
       <c r="K6" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" t="s">
-        <v>73</v>
+      <c r="C7" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -872,16 +1096,55 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="L7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="X7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="5"/>
+      <c r="C8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="12"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
         <v>29</v>
@@ -893,16 +1156,51 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="L8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD8" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="5"/>
+      <c r="C9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="12"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
         <v>30</v>
@@ -914,16 +1212,35 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="5"/>
+      <c r="C10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="12"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
         <v>31</v>
@@ -935,16 +1252,35 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="5"/>
+      <c r="C11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
         <v>32</v>
@@ -956,16 +1292,35 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="C12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
         <v>33</v>
@@ -977,19 +1332,38 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
-        <v>79</v>
+      <c r="C13" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1002,17 +1376,36 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" t="s">
-        <v>80</v>
+      <c r="C14" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1025,17 +1418,36 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" t="s">
-        <v>81</v>
+      <c r="C15" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1048,17 +1460,36 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" t="s">
-        <v>82</v>
+      <c r="C16" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1071,17 +1502,36 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" t="s">
-        <v>83</v>
+      <c r="C17" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1094,16 +1544,35 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="5"/>
+      <c r="C18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="2"/>
       <c r="F18" s="7" t="s">
         <v>36</v>
@@ -1115,18 +1584,37 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="5"/>
+      <c r="C19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="2"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
@@ -1138,16 +1626,35 @@
       <c r="K19" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="5"/>
+      <c r="C20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="2"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
@@ -1159,16 +1666,35 @@
       <c r="K20" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="5"/>
+      <c r="C21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="2"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
@@ -1180,18 +1706,37 @@
       <c r="K21" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row ht="26.25" r="22" spans="1:11">
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+    </row>
+    <row r="22" spans="1:30" ht="26.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="5"/>
+      <c r="C22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
         <v>22</v>
@@ -1203,9 +1748,28 @@
       <c r="K22" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row ht="26.25" r="23" spans="1:11">
-      <c r="A23" s="8">
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+    </row>
+    <row r="23" spans="1:30" ht="26.25">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
@@ -1222,8 +1786,27 @@
       <c r="K23" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="5"/>
@@ -1235,9 +1818,28 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 4th May 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" tabRatio="614"/>
+    <workbookView tabRatio="614" windowHeight="9660" windowWidth="19815" xWindow="390" yWindow="510"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="142">
   <si>
     <t>Sno</t>
   </si>
@@ -248,6 +248,198 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>320018447104</t>
+  </si>
+  <si>
+    <t>320018447115</t>
+  </si>
+  <si>
+    <t>320018447148</t>
+  </si>
+  <si>
+    <t>320018447160</t>
+  </si>
+  <si>
+    <t>320018447207</t>
+  </si>
+  <si>
+    <t>320018447229</t>
+  </si>
+  <si>
+    <t>320018447251</t>
+  </si>
+  <si>
+    <t>320018447273</t>
+  </si>
+  <si>
+    <t>320018447300</t>
+  </si>
+  <si>
+    <t>320018447321</t>
+  </si>
+  <si>
+    <t>320018447365</t>
+  </si>
+  <si>
+    <t>320018447387</t>
+  </si>
+  <si>
+    <t>320018447413</t>
+  </si>
+  <si>
+    <t>320018447435</t>
+  </si>
+  <si>
+    <t>320018447468</t>
+  </si>
+  <si>
+    <t>320018447480</t>
+  </si>
+  <si>
+    <t>320018447527</t>
+  </si>
+  <si>
+    <t>320018447549</t>
+  </si>
+  <si>
+    <t>320018447571</t>
+  </si>
+  <si>
+    <t>320018447593</t>
+  </si>
+  <si>
+    <t>320018447620</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>320018457870</t>
+  </si>
+  <si>
+    <t>320018457881</t>
+  </si>
+  <si>
+    <t>320018457918</t>
+  </si>
+  <si>
+    <t>320018457930</t>
+  </si>
+  <si>
+    <t>320018457973</t>
+  </si>
+  <si>
+    <t>320018457995</t>
+  </si>
+  <si>
+    <t>320018458020</t>
+  </si>
+  <si>
+    <t>320018458042</t>
+  </si>
+  <si>
+    <t>320018458075</t>
+  </si>
+  <si>
+    <t>320018458097</t>
+  </si>
+  <si>
+    <t>320018458134</t>
+  </si>
+  <si>
+    <t>320018458156</t>
+  </si>
+  <si>
+    <t>320018458189</t>
+  </si>
+  <si>
+    <t>320018458204</t>
+  </si>
+  <si>
+    <t>320018458237</t>
+  </si>
+  <si>
+    <t>320018458259</t>
+  </si>
+  <si>
+    <t>320018458292</t>
+  </si>
+  <si>
+    <t>320018458318</t>
+  </si>
+  <si>
+    <t>320018458340</t>
+  </si>
+  <si>
+    <t>320018458362</t>
+  </si>
+  <si>
+    <t>320018458395</t>
+  </si>
+  <si>
+    <t>320018464460</t>
+  </si>
+  <si>
+    <t>320018464471</t>
+  </si>
+  <si>
+    <t>320018464508</t>
+  </si>
+  <si>
+    <t>320018464520</t>
+  </si>
+  <si>
+    <t>320018464563</t>
+  </si>
+  <si>
+    <t>320018464585</t>
+  </si>
+  <si>
+    <t>320018464611</t>
+  </si>
+  <si>
+    <t>320018464633</t>
+  </si>
+  <si>
+    <t>320018464666</t>
+  </si>
+  <si>
+    <t>320018464688</t>
+  </si>
+  <si>
+    <t>320018464725</t>
+  </si>
+  <si>
+    <t>320018464747</t>
+  </si>
+  <si>
+    <t>320018464770</t>
+  </si>
+  <si>
+    <t>320018464791</t>
+  </si>
+  <si>
+    <t>320018464828</t>
+  </si>
+  <si>
+    <t>320018464840</t>
+  </si>
+  <si>
+    <t>320018464883</t>
+  </si>
+  <si>
+    <t>320018464909</t>
+  </si>
+  <si>
+    <t>320018464931</t>
+  </si>
+  <si>
+    <t>320018464953</t>
+  </si>
+  <si>
+    <t>320018464986</t>
   </si>
 </sst>
 </file>
@@ -352,49 +544,49 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -408,10 +600,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -569,7 +761,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -578,13 +770,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -594,7 +786,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -603,7 +795,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -612,7 +804,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -622,12 +814,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -658,7 +850,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -677,7 +869,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -689,7 +881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -698,33 +890,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="104.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="104.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39">
+    <row ht="39" r="1" spans="1:30">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -823,8 +1015,8 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>57</v>
+      <c r="C2" t="s">
+        <v>121</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -836,19 +1028,19 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="11" t="s">
+      <c r="L2" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" t="s">
         <v>77</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" t="s">
         <v>77</v>
       </c>
       <c r="Q2" s="11"/>
@@ -866,15 +1058,15 @@
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>
     </row>
-    <row r="3" spans="1:30" ht="14.25" customHeight="1">
+    <row customHeight="1" ht="14.25" r="3" spans="1:30">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
+      <c r="C3" t="s">
+        <v>122</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -891,8 +1083,8 @@
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
-      <c r="Q3" s="11" t="s">
-        <v>77</v>
+      <c r="Q3" t="s">
+        <v>99</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -915,8 +1107,8 @@
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>59</v>
+      <c r="C4" t="s">
+        <v>123</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -931,20 +1123,20 @@
         <v>26</v>
       </c>
       <c r="L4" s="11"/>
-      <c r="M4" s="11" t="s">
+      <c r="M4" t="s">
         <v>76</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" t="s">
         <v>77</v>
       </c>
       <c r="Q4" s="11"/>
-      <c r="R4" s="11" t="s">
+      <c r="R4" t="s">
         <v>77</v>
       </c>
       <c r="S4" s="11"/>
@@ -967,11 +1159,11 @@
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>60</v>
+      <c r="C5" t="s">
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -985,21 +1177,21 @@
         <v>20</v>
       </c>
       <c r="L5" s="11"/>
-      <c r="M5" s="11" t="s">
+      <c r="M5" t="s">
         <v>76</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" t="s">
         <v>77</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" t="s">
         <v>77</v>
       </c>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="S5" s="11" t="s">
+      <c r="S5" t="s">
         <v>77</v>
       </c>
       <c r="T5" s="11"/>
@@ -1021,11 +1213,11 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>61</v>
+      <c r="C6" t="s">
+        <v>125</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1040,27 +1232,27 @@
       <c r="K6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" t="s">
         <v>76</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" t="s">
         <v>77</v>
       </c>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
-      <c r="S6" s="11" t="s">
+      <c r="S6" t="s">
         <v>76</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="T6" t="s">
         <v>76</v>
       </c>
       <c r="U6" s="11"/>
@@ -1079,11 +1271,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="6" t="s">
-        <v>62</v>
+      <c r="C7" t="s">
+        <v>126</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1096,38 +1288,38 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="11" t="s">
+      <c r="L7" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O7" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="P7" t="s">
         <v>77</v>
       </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
-      <c r="U7" s="11" t="s">
+      <c r="U7" t="s">
         <v>76</v>
       </c>
-      <c r="V7" s="11" t="s">
+      <c r="V7" t="s">
         <v>76</v>
       </c>
-      <c r="W7" s="11" t="s">
+      <c r="W7" t="s">
         <v>76</v>
       </c>
-      <c r="X7" s="11" t="s">
+      <c r="X7" t="s">
         <v>76</v>
       </c>
-      <c r="Y7" s="11" t="s">
+      <c r="Y7" t="s">
         <v>76</v>
       </c>
       <c r="Z7" s="11"/>
@@ -1141,8 +1333,8 @@
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="6" t="s">
-        <v>63</v>
+      <c r="C8" t="s">
+        <v>127</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -1156,19 +1348,19 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="11" t="s">
+      <c r="L8" t="s">
         <v>76</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" t="s">
         <v>76</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" t="s">
         <v>77</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" t="s">
         <v>77</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="P8" t="s">
         <v>77</v>
       </c>
       <c r="Q8" s="11"/>
@@ -1182,13 +1374,13 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
       <c r="AA8" s="11"/>
-      <c r="AB8" s="11" t="s">
+      <c r="AB8" t="s">
         <v>77</v>
       </c>
-      <c r="AC8" s="11" t="s">
+      <c r="AC8" t="s">
         <v>76</v>
       </c>
-      <c r="AD8" s="11" t="s">
+      <c r="AD8" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1197,8 +1389,8 @@
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="6" t="s">
-        <v>64</v>
+      <c r="C9" t="s">
+        <v>128</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -1237,8 +1429,8 @@
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="6" t="s">
-        <v>65</v>
+      <c r="C10" t="s">
+        <v>129</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -1277,8 +1469,8 @@
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="6" t="s">
-        <v>66</v>
+      <c r="C11" t="s">
+        <v>130</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -1317,8 +1509,8 @@
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
-        <v>67</v>
+      <c r="C12" t="s">
+        <v>131</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -1359,11 +1551,11 @@
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>68</v>
+      <c r="C13" t="s">
+        <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1401,11 +1593,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="6" t="s">
-        <v>69</v>
+      <c r="C14" t="s">
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1443,11 +1635,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="6" t="s">
-        <v>70</v>
+      <c r="C15" t="s">
+        <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>134</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1485,11 +1677,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="6" t="s">
-        <v>71</v>
+      <c r="C16" t="s">
+        <v>135</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1527,11 +1719,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="6" t="s">
-        <v>72</v>
+      <c r="C17" t="s">
+        <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1569,8 +1761,8 @@
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="6" t="s">
-        <v>73</v>
+      <c r="C18" t="s">
+        <v>137</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -1611,8 +1803,8 @@
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>74</v>
+      <c r="C19" t="s">
+        <v>138</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -1651,8 +1843,8 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="6" t="s">
-        <v>75</v>
+      <c r="C20" t="s">
+        <v>139</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -1691,8 +1883,8 @@
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="6" t="s">
-        <v>55</v>
+      <c r="C21" t="s">
+        <v>140</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -1726,15 +1918,15 @@
       <c r="AC21" s="11"/>
       <c r="AD21" s="11"/>
     </row>
-    <row r="22" spans="1:30" ht="26.25">
+    <row ht="26.25" r="22" spans="1:30">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>56</v>
+      <c r="C22" t="s">
+        <v>141</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>
@@ -1768,7 +1960,7 @@
       <c r="AC22" s="11"/>
       <c r="AD22" s="11"/>
     </row>
-    <row r="23" spans="1:30" ht="26.25">
+    <row ht="26.25" r="23" spans="1:30">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1839,7 +2031,7 @@
       <c r="AD24" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 5th May 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="164">
   <si>
     <t>Sno</t>
   </si>
@@ -440,6 +440,72 @@
   </si>
   <si>
     <t>320018464986</t>
+  </si>
+  <si>
+    <t>320018465044</t>
+  </si>
+  <si>
+    <t>320018471602</t>
+  </si>
+  <si>
+    <t>320018471613</t>
+  </si>
+  <si>
+    <t>320018471646</t>
+  </si>
+  <si>
+    <t>320018471668</t>
+  </si>
+  <si>
+    <t>320018471705</t>
+  </si>
+  <si>
+    <t>320018471727</t>
+  </si>
+  <si>
+    <t>320018471750</t>
+  </si>
+  <si>
+    <t>320018471771</t>
+  </si>
+  <si>
+    <t>320018471808</t>
+  </si>
+  <si>
+    <t>320018471820</t>
+  </si>
+  <si>
+    <t>320018471863</t>
+  </si>
+  <si>
+    <t>320018471885</t>
+  </si>
+  <si>
+    <t>320018471911</t>
+  </si>
+  <si>
+    <t>320018471933</t>
+  </si>
+  <si>
+    <t>320018471966</t>
+  </si>
+  <si>
+    <t>320018471988</t>
+  </si>
+  <si>
+    <t>320018472024</t>
+  </si>
+  <si>
+    <t>320018472046</t>
+  </si>
+  <si>
+    <t>320018472079</t>
+  </si>
+  <si>
+    <t>320018472090</t>
+  </si>
+  <si>
+    <t>320018472127</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1082,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1066,7 +1132,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -1108,7 +1174,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -1160,10 +1226,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1214,10 +1280,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1272,10 +1338,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1334,7 +1400,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -1390,7 +1456,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -1430,7 +1496,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -1470,7 +1536,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -1510,7 +1576,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -1552,10 +1618,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1594,10 +1660,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1636,10 +1702,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1678,10 +1744,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1720,10 +1786,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1762,7 +1828,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -1804,7 +1870,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -1844,7 +1910,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -1884,7 +1950,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -1926,7 +1992,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 19th May 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="385">
   <si>
     <t>Sno</t>
   </si>
@@ -881,6 +881,294 @@
   </si>
   <si>
     <t>320017959366</t>
+  </si>
+  <si>
+    <t>320018573159</t>
+  </si>
+  <si>
+    <t>320018573170</t>
+  </si>
+  <si>
+    <t>320018573207</t>
+  </si>
+  <si>
+    <t>320018573229</t>
+  </si>
+  <si>
+    <t>320018573262</t>
+  </si>
+  <si>
+    <t>320018573284</t>
+  </si>
+  <si>
+    <t>320018573310</t>
+  </si>
+  <si>
+    <t>320018575140</t>
+  </si>
+  <si>
+    <t>320018575151</t>
+  </si>
+  <si>
+    <t>320018575184</t>
+  </si>
+  <si>
+    <t>320018575200</t>
+  </si>
+  <si>
+    <t>320018575243</t>
+  </si>
+  <si>
+    <t>320018575265</t>
+  </si>
+  <si>
+    <t>320018575298</t>
+  </si>
+  <si>
+    <t>320018575313</t>
+  </si>
+  <si>
+    <t>320018575346</t>
+  </si>
+  <si>
+    <t>320018575368</t>
+  </si>
+  <si>
+    <t>320018575405</t>
+  </si>
+  <si>
+    <t>320018575427</t>
+  </si>
+  <si>
+    <t>320018575450</t>
+  </si>
+  <si>
+    <t>320018575519</t>
+  </si>
+  <si>
+    <t>320018575520</t>
+  </si>
+  <si>
+    <t>320018575552</t>
+  </si>
+  <si>
+    <t>320018575574</t>
+  </si>
+  <si>
+    <t>320018575611</t>
+  </si>
+  <si>
+    <t>320018575633</t>
+  </si>
+  <si>
+    <t>320018575666</t>
+  </si>
+  <si>
+    <t>320018575688</t>
+  </si>
+  <si>
+    <t>320018575714</t>
+  </si>
+  <si>
+    <t>320018575736</t>
+  </si>
+  <si>
+    <t>320018575770</t>
+  </si>
+  <si>
+    <t>320018575791</t>
+  </si>
+  <si>
+    <t>320018575828</t>
+  </si>
+  <si>
+    <t>320018579146</t>
+  </si>
+  <si>
+    <t>320018579157</t>
+  </si>
+  <si>
+    <t>320018579180</t>
+  </si>
+  <si>
+    <t>320018579190</t>
+  </si>
+  <si>
+    <t>320018579216</t>
+  </si>
+  <si>
+    <t>320018579249</t>
+  </si>
+  <si>
+    <t>320018579282</t>
+  </si>
+  <si>
+    <t>320018579308</t>
+  </si>
+  <si>
+    <t>320018579341</t>
+  </si>
+  <si>
+    <t>320018579363</t>
+  </si>
+  <si>
+    <t>320018579385</t>
+  </si>
+  <si>
+    <t>320018579411</t>
+  </si>
+  <si>
+    <t>320018579444</t>
+  </si>
+  <si>
+    <t>320018579477</t>
+  </si>
+  <si>
+    <t>320018579499</t>
+  </si>
+  <si>
+    <t>320018579525</t>
+  </si>
+  <si>
+    <t>320018579558</t>
+  </si>
+  <si>
+    <t>320018579570</t>
+  </si>
+  <si>
+    <t>320018579591</t>
+  </si>
+  <si>
+    <t>320018579639</t>
+  </si>
+  <si>
+    <t>320018579672</t>
+  </si>
+  <si>
+    <t>320018579694</t>
+  </si>
+  <si>
+    <t>320018579710</t>
+  </si>
+  <si>
+    <t>320018579742</t>
+  </si>
+  <si>
+    <t>320018579775</t>
+  </si>
+  <si>
+    <t>320018579797</t>
+  </si>
+  <si>
+    <t>320018579812</t>
+  </si>
+  <si>
+    <t>320018579845</t>
+  </si>
+  <si>
+    <t>320018579889</t>
+  </si>
+  <si>
+    <t>320018579904</t>
+  </si>
+  <si>
+    <t>320018579926</t>
+  </si>
+  <si>
+    <t>320018579981</t>
+  </si>
+  <si>
+    <t>320018580025</t>
+  </si>
+  <si>
+    <t>320018580047</t>
+  </si>
+  <si>
+    <t>320018580070</t>
+  </si>
+  <si>
+    <t>320018580106</t>
+  </si>
+  <si>
+    <t>320018580139</t>
+  </si>
+  <si>
+    <t>320018580150</t>
+  </si>
+  <si>
+    <t>320018580172</t>
+  </si>
+  <si>
+    <t>320018580209</t>
+  </si>
+  <si>
+    <t>320018580231</t>
+  </si>
+  <si>
+    <t>320018580242</t>
+  </si>
+  <si>
+    <t>320018582988</t>
+  </si>
+  <si>
+    <t>320018583002</t>
+  </si>
+  <si>
+    <t>320018583035</t>
+  </si>
+  <si>
+    <t>320018583057</t>
+  </si>
+  <si>
+    <t>320018583090</t>
+  </si>
+  <si>
+    <t>320018583116</t>
+  </si>
+  <si>
+    <t>320018583149</t>
+  </si>
+  <si>
+    <t>320018583160</t>
+  </si>
+  <si>
+    <t>320018583193</t>
+  </si>
+  <si>
+    <t>320018583219</t>
+  </si>
+  <si>
+    <t>320018583285</t>
+  </si>
+  <si>
+    <t>320018583300</t>
+  </si>
+  <si>
+    <t>320018583333</t>
+  </si>
+  <si>
+    <t>320018583355</t>
+  </si>
+  <si>
+    <t>320018583388</t>
+  </si>
+  <si>
+    <t>320018583403</t>
+  </si>
+  <si>
+    <t>320018583470</t>
+  </si>
+  <si>
+    <t>320018583701</t>
+  </si>
+  <si>
+    <t>320018583734</t>
+  </si>
+  <si>
+    <t>320018583756</t>
+  </si>
+  <si>
+    <t>320018583789</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1745,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>364</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1476,13 +1764,13 @@
         <v>76</v>
       </c>
       <c r="N2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
@@ -1507,7 +1795,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>269</v>
+        <v>365</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -1525,7 +1813,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -1549,7 +1837,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>366</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -1568,17 +1856,17 @@
         <v>76</v>
       </c>
       <c r="N4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
@@ -1601,10 +1889,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>367</v>
       </c>
       <c r="D5" t="s">
-        <v>271</v>
+        <v>367</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1622,18 +1910,18 @@
         <v>76</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
@@ -1655,10 +1943,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>368</v>
       </c>
       <c r="D6" t="s">
-        <v>272</v>
+        <v>368</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1680,13 +1968,13 @@
         <v>76</v>
       </c>
       <c r="N6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
@@ -1713,10 +2001,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>369</v>
       </c>
       <c r="D7" t="s">
-        <v>273</v>
+        <v>369</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1736,18 +2024,20 @@
         <v>76</v>
       </c>
       <c r="N7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+      <c r="T7" t="s">
+        <v>76</v>
+      </c>
       <c r="U7" t="s">
         <v>76</v>
       </c>
@@ -1775,7 +2065,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>274</v>
+        <v>370</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -1831,7 +2121,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>275</v>
+        <v>371</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -1871,7 +2161,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>276</v>
+        <v>372</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -1911,7 +2201,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>277</v>
+        <v>373</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -1951,7 +2241,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>278</v>
+        <v>374</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -1993,10 +2283,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>279</v>
+        <v>375</v>
       </c>
       <c r="D13" t="s">
-        <v>279</v>
+        <v>375</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2009,16 +2299,28 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
+      <c r="L13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" t="s">
+        <v>76</v>
+      </c>
+      <c r="P13" t="s">
+        <v>76</v>
+      </c>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
+      <c r="U13" t="s">
+        <v>76</v>
+      </c>
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
       <c r="X13" s="11"/>
@@ -2035,10 +2337,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>280</v>
+        <v>376</v>
       </c>
       <c r="D14" t="s">
-        <v>280</v>
+        <v>376</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2051,17 +2353,29 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
+      <c r="L14" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" t="s">
+        <v>76</v>
+      </c>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
+      <c r="V14" t="s">
+        <v>76</v>
+      </c>
       <c r="W14" s="11"/>
       <c r="X14" s="11"/>
       <c r="Y14" s="11"/>
@@ -2077,10 +2391,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>281</v>
+        <v>377</v>
       </c>
       <c r="D15" t="s">
-        <v>281</v>
+        <v>377</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2093,18 +2407,30 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
+      <c r="L15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15" t="s">
+        <v>76</v>
+      </c>
+      <c r="P15" t="s">
+        <v>76</v>
+      </c>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
+      <c r="W15" t="s">
+        <v>76</v>
+      </c>
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="11"/>
@@ -2119,10 +2445,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>282</v>
+        <v>378</v>
       </c>
       <c r="D16" t="s">
-        <v>282</v>
+        <v>378</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2135,11 +2461,21 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
+      <c r="L16" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" t="s">
+        <v>76</v>
+      </c>
+      <c r="N16" t="s">
+        <v>76</v>
+      </c>
+      <c r="O16" t="s">
+        <v>76</v>
+      </c>
+      <c r="P16" t="s">
+        <v>76</v>
+      </c>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
@@ -2147,7 +2483,9 @@
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
+      <c r="X16" t="s">
+        <v>76</v>
+      </c>
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
       <c r="AA16" s="11"/>
@@ -2161,10 +2499,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>283</v>
+        <v>379</v>
       </c>
       <c r="D17" t="s">
-        <v>283</v>
+        <v>379</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2177,11 +2515,21 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="L17" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17" t="s">
+        <v>76</v>
+      </c>
+      <c r="O17" t="s">
+        <v>76</v>
+      </c>
+      <c r="P17" t="s">
+        <v>76</v>
+      </c>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
@@ -2190,7 +2538,9 @@
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
+      <c r="Y17" t="s">
+        <v>76</v>
+      </c>
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
       <c r="AB17" s="11"/>
@@ -2203,7 +2553,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>284</v>
+        <v>380</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -2245,7 +2595,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>285</v>
+        <v>381</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -2259,11 +2609,21 @@
       <c r="K19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
+      <c r="L19" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N19" t="s">
+        <v>76</v>
+      </c>
+      <c r="O19" t="s">
+        <v>76</v>
+      </c>
+      <c r="P19" t="s">
+        <v>76</v>
+      </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
@@ -2275,7 +2635,9 @@
       <c r="Y19" s="11"/>
       <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
+      <c r="AB19" t="s">
+        <v>76</v>
+      </c>
       <c r="AC19" s="11"/>
       <c r="AD19" s="11"/>
     </row>
@@ -2285,7 +2647,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>286</v>
+        <v>382</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -2299,11 +2661,21 @@
       <c r="K20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
+      <c r="L20" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N20" t="s">
+        <v>76</v>
+      </c>
+      <c r="O20" t="s">
+        <v>76</v>
+      </c>
+      <c r="P20" t="s">
+        <v>76</v>
+      </c>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
@@ -2316,7 +2688,9 @@
       <c r="Z20" s="11"/>
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
-      <c r="AC20" s="11"/>
+      <c r="AC20" t="s">
+        <v>76</v>
+      </c>
       <c r="AD20" s="11"/>
     </row>
     <row r="21" spans="1:30">
@@ -2325,7 +2699,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>287</v>
+        <v>383</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -2339,11 +2713,21 @@
       <c r="K21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
+      <c r="L21" t="s">
+        <v>76</v>
+      </c>
+      <c r="M21" t="s">
+        <v>76</v>
+      </c>
+      <c r="N21" t="s">
+        <v>76</v>
+      </c>
+      <c r="O21" t="s">
+        <v>76</v>
+      </c>
+      <c r="P21" t="s">
+        <v>76</v>
+      </c>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
@@ -2357,7 +2741,9 @@
       <c r="AA21" s="11"/>
       <c r="AB21" s="11"/>
       <c r="AC21" s="11"/>
-      <c r="AD21" s="11"/>
+      <c r="AD21" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row ht="26.25" r="22" spans="1:30">
       <c r="A22" s="3">
@@ -2367,7 +2753,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>288</v>
+        <v>384</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Final changes for cheetah
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2559" uniqueCount="406">
   <si>
     <t>Sno</t>
   </si>
@@ -1169,6 +1169,69 @@
   </si>
   <si>
     <t>320018583789</t>
+  </si>
+  <si>
+    <t>320018586090</t>
+  </si>
+  <si>
+    <t>320018586104</t>
+  </si>
+  <si>
+    <t>320018586137</t>
+  </si>
+  <si>
+    <t>320018586159</t>
+  </si>
+  <si>
+    <t>320018586192</t>
+  </si>
+  <si>
+    <t>320018586218</t>
+  </si>
+  <si>
+    <t>320018586240</t>
+  </si>
+  <si>
+    <t>320018586262</t>
+  </si>
+  <si>
+    <t>320018586295</t>
+  </si>
+  <si>
+    <t>320018586310</t>
+  </si>
+  <si>
+    <t>320018586354</t>
+  </si>
+  <si>
+    <t>320018586376</t>
+  </si>
+  <si>
+    <t>320018586402</t>
+  </si>
+  <si>
+    <t>320018586424</t>
+  </si>
+  <si>
+    <t>320018586457</t>
+  </si>
+  <si>
+    <t>320018586479</t>
+  </si>
+  <si>
+    <t>320018586516</t>
+  </si>
+  <si>
+    <t>320018586538</t>
+  </si>
+  <si>
+    <t>320018586560</t>
+  </si>
+  <si>
+    <t>320018586582</t>
+  </si>
+  <si>
+    <t>320018586619</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -1745,7 +1808,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>364</v>
+        <v>385</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1795,7 +1858,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>365</v>
+        <v>386</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -1837,7 +1900,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>366</v>
+        <v>387</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -1889,10 +1952,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>367</v>
+        <v>388</v>
       </c>
       <c r="D5" t="s">
-        <v>367</v>
+        <v>388</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1943,10 +2006,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>368</v>
+        <v>389</v>
       </c>
       <c r="D6" t="s">
-        <v>368</v>
+        <v>389</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -2001,10 +2064,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
       <c r="D7" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -2065,7 +2128,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>370</v>
+        <v>391</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -2121,7 +2184,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>371</v>
+        <v>392</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -2161,7 +2224,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>372</v>
+        <v>393</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -2201,7 +2264,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>373</v>
+        <v>394</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -2241,7 +2304,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>374</v>
+        <v>395</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -2283,10 +2346,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
       <c r="D13" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2337,10 +2400,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="D14" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2391,10 +2454,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>377</v>
+        <v>398</v>
       </c>
       <c r="D15" t="s">
-        <v>377</v>
+        <v>398</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2445,10 +2508,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>378</v>
+        <v>399</v>
       </c>
       <c r="D16" t="s">
-        <v>378</v>
+        <v>399</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2499,10 +2562,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>379</v>
+        <v>400</v>
       </c>
       <c r="D17" t="s">
-        <v>379</v>
+        <v>400</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2553,7 +2616,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>380</v>
+        <v>401</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -2595,7 +2658,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -2647,7 +2710,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>382</v>
+        <v>403</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -2699,7 +2762,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>383</v>
+        <v>404</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -2753,7 +2816,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>384</v>
+        <v>405</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of DEV URL configuration
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2559" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4449" uniqueCount="827">
   <si>
     <t>Sno</t>
   </si>
@@ -1232,6 +1232,1269 @@
   </si>
   <si>
     <t>320018586619</t>
+  </si>
+  <si>
+    <t>320018606316</t>
+  </si>
+  <si>
+    <t>320018606327</t>
+  </si>
+  <si>
+    <t>320018606350</t>
+  </si>
+  <si>
+    <t>320018606371</t>
+  </si>
+  <si>
+    <t>320018606419</t>
+  </si>
+  <si>
+    <t>320018606430</t>
+  </si>
+  <si>
+    <t>320018606463</t>
+  </si>
+  <si>
+    <t>320018606485</t>
+  </si>
+  <si>
+    <t>320018606511</t>
+  </si>
+  <si>
+    <t>320018606533</t>
+  </si>
+  <si>
+    <t>320018606577</t>
+  </si>
+  <si>
+    <t>320018606599</t>
+  </si>
+  <si>
+    <t>320018606625</t>
+  </si>
+  <si>
+    <t>320018606647</t>
+  </si>
+  <si>
+    <t>320018606670</t>
+  </si>
+  <si>
+    <t>320018606691</t>
+  </si>
+  <si>
+    <t>320018606739</t>
+  </si>
+  <si>
+    <t>320018606750</t>
+  </si>
+  <si>
+    <t>320018606783</t>
+  </si>
+  <si>
+    <t>320018606809</t>
+  </si>
+  <si>
+    <t>320018606831</t>
+  </si>
+  <si>
+    <t>320018621062</t>
+  </si>
+  <si>
+    <t>320018621073</t>
+  </si>
+  <si>
+    <t>320018621100</t>
+  </si>
+  <si>
+    <t>320018621121</t>
+  </si>
+  <si>
+    <t>320018621165</t>
+  </si>
+  <si>
+    <t>320018621187</t>
+  </si>
+  <si>
+    <t>320018621213</t>
+  </si>
+  <si>
+    <t>320018621235</t>
+  </si>
+  <si>
+    <t>320018621268</t>
+  </si>
+  <si>
+    <t>320018621280</t>
+  </si>
+  <si>
+    <t>320018621327</t>
+  </si>
+  <si>
+    <t>320018621349</t>
+  </si>
+  <si>
+    <t>320018621371</t>
+  </si>
+  <si>
+    <t>320018621393</t>
+  </si>
+  <si>
+    <t>320018621420</t>
+  </si>
+  <si>
+    <t>320018621441</t>
+  </si>
+  <si>
+    <t>320018621485</t>
+  </si>
+  <si>
+    <t>320018621500</t>
+  </si>
+  <si>
+    <t>320018621533</t>
+  </si>
+  <si>
+    <t>320018621555</t>
+  </si>
+  <si>
+    <t>320018621588</t>
+  </si>
+  <si>
+    <t>320018624006</t>
+  </si>
+  <si>
+    <t>320018624657</t>
+  </si>
+  <si>
+    <t>320018624922</t>
+  </si>
+  <si>
+    <t>320018624933</t>
+  </si>
+  <si>
+    <t>320018624966</t>
+  </si>
+  <si>
+    <t>320018624988</t>
+  </si>
+  <si>
+    <t>320018625024</t>
+  </si>
+  <si>
+    <t>320018625046</t>
+  </si>
+  <si>
+    <t>320018625079</t>
+  </si>
+  <si>
+    <t>320018625090</t>
+  </si>
+  <si>
+    <t>320018625127</t>
+  </si>
+  <si>
+    <t>320018625149</t>
+  </si>
+  <si>
+    <t>320018625182</t>
+  </si>
+  <si>
+    <t>320018625220</t>
+  </si>
+  <si>
+    <t>320018625252</t>
+  </si>
+  <si>
+    <t>320018625274</t>
+  </si>
+  <si>
+    <t>320018625300</t>
+  </si>
+  <si>
+    <t>320018625322</t>
+  </si>
+  <si>
+    <t>320018625366</t>
+  </si>
+  <si>
+    <t>320018625388</t>
+  </si>
+  <si>
+    <t>320018625414</t>
+  </si>
+  <si>
+    <t>320018625436</t>
+  </si>
+  <si>
+    <t>320018625469</t>
+  </si>
+  <si>
+    <t>320018628560</t>
+  </si>
+  <si>
+    <t>320018628571</t>
+  </si>
+  <si>
+    <t>320018628608</t>
+  </si>
+  <si>
+    <t>320018628620</t>
+  </si>
+  <si>
+    <t>320018628663</t>
+  </si>
+  <si>
+    <t>320018628685</t>
+  </si>
+  <si>
+    <t>320018628711</t>
+  </si>
+  <si>
+    <t>320018628733</t>
+  </si>
+  <si>
+    <t>320018628766</t>
+  </si>
+  <si>
+    <t>320018628788</t>
+  </si>
+  <si>
+    <t>320018628825</t>
+  </si>
+  <si>
+    <t>320018628847</t>
+  </si>
+  <si>
+    <t>320018628870</t>
+  </si>
+  <si>
+    <t>320018630457</t>
+  </si>
+  <si>
+    <t>320018630468</t>
+  </si>
+  <si>
+    <t>320018630490</t>
+  </si>
+  <si>
+    <t>320018630733</t>
+  </si>
+  <si>
+    <t>320018630777</t>
+  </si>
+  <si>
+    <t>320018630799</t>
+  </si>
+  <si>
+    <t>320018630825</t>
+  </si>
+  <si>
+    <t>320018630847</t>
+  </si>
+  <si>
+    <t>320018630870</t>
+  </si>
+  <si>
+    <t>320018630891</t>
+  </si>
+  <si>
+    <t>320018630939</t>
+  </si>
+  <si>
+    <t>320018630950</t>
+  </si>
+  <si>
+    <t>320018630983</t>
+  </si>
+  <si>
+    <t>320018631008</t>
+  </si>
+  <si>
+    <t>320018631030</t>
+  </si>
+  <si>
+    <t>320018631063</t>
+  </si>
+  <si>
+    <t>320018631100</t>
+  </si>
+  <si>
+    <t>320018631133</t>
+  </si>
+  <si>
+    <t>320018631177</t>
+  </si>
+  <si>
+    <t>320018631199</t>
+  </si>
+  <si>
+    <t>320018631225</t>
+  </si>
+  <si>
+    <t>320018638745</t>
+  </si>
+  <si>
+    <t>320018638756</t>
+  </si>
+  <si>
+    <t>320018638789</t>
+  </si>
+  <si>
+    <t>320018638804</t>
+  </si>
+  <si>
+    <t>320018638848</t>
+  </si>
+  <si>
+    <t>320018638860</t>
+  </si>
+  <si>
+    <t>320018638892</t>
+  </si>
+  <si>
+    <t>320018638918</t>
+  </si>
+  <si>
+    <t>320018638940</t>
+  </si>
+  <si>
+    <t>320018638962</t>
+  </si>
+  <si>
+    <t>320018639009</t>
+  </si>
+  <si>
+    <t>320018639020</t>
+  </si>
+  <si>
+    <t>320018639053</t>
+  </si>
+  <si>
+    <t>320018639075</t>
+  </si>
+  <si>
+    <t>320018639101</t>
+  </si>
+  <si>
+    <t>320018639123</t>
+  </si>
+  <si>
+    <t>320018639167</t>
+  </si>
+  <si>
+    <t>320018639189</t>
+  </si>
+  <si>
+    <t>320018639215</t>
+  </si>
+  <si>
+    <t>320018639237</t>
+  </si>
+  <si>
+    <t>320018639260</t>
+  </si>
+  <si>
+    <t>320018648963</t>
+  </si>
+  <si>
+    <t>320018648996</t>
+  </si>
+  <si>
+    <t>320018649021</t>
+  </si>
+  <si>
+    <t>320018649065</t>
+  </si>
+  <si>
+    <t>320018649098</t>
+  </si>
+  <si>
+    <t>320018649135</t>
+  </si>
+  <si>
+    <t>320018649157</t>
+  </si>
+  <si>
+    <t>320018649190</t>
+  </si>
+  <si>
+    <t>320018649216</t>
+  </si>
+  <si>
+    <t>320018649250</t>
+  </si>
+  <si>
+    <t>320018649271</t>
+  </si>
+  <si>
+    <t>320018649319</t>
+  </si>
+  <si>
+    <t>320018649330</t>
+  </si>
+  <si>
+    <t>320018649363</t>
+  </si>
+  <si>
+    <t>320018649385</t>
+  </si>
+  <si>
+    <t>320018649411</t>
+  </si>
+  <si>
+    <t>320018679826</t>
+  </si>
+  <si>
+    <t>320018679837</t>
+  </si>
+  <si>
+    <t>320018679860</t>
+  </si>
+  <si>
+    <t>320018679881</t>
+  </si>
+  <si>
+    <t>320018679929</t>
+  </si>
+  <si>
+    <t>320018679940</t>
+  </si>
+  <si>
+    <t>320018679973</t>
+  </si>
+  <si>
+    <t>320018679995</t>
+  </si>
+  <si>
+    <t>320018680028</t>
+  </si>
+  <si>
+    <t>320018680040</t>
+  </si>
+  <si>
+    <t>320018680083</t>
+  </si>
+  <si>
+    <t>320018680109</t>
+  </si>
+  <si>
+    <t>320018680131</t>
+  </si>
+  <si>
+    <t>320018680153</t>
+  </si>
+  <si>
+    <t>320018680186</t>
+  </si>
+  <si>
+    <t>320018680201</t>
+  </si>
+  <si>
+    <t>320018680245</t>
+  </si>
+  <si>
+    <t>320018680278</t>
+  </si>
+  <si>
+    <t>320018680304</t>
+  </si>
+  <si>
+    <t>320018680326</t>
+  </si>
+  <si>
+    <t>320018680359</t>
+  </si>
+  <si>
+    <t>320018686585</t>
+  </si>
+  <si>
+    <t>320018686596</t>
+  </si>
+  <si>
+    <t>320018686622</t>
+  </si>
+  <si>
+    <t>320018686644</t>
+  </si>
+  <si>
+    <t>320018686688</t>
+  </si>
+  <si>
+    <t>320018686703</t>
+  </si>
+  <si>
+    <t>320018686736</t>
+  </si>
+  <si>
+    <t>320018686758</t>
+  </si>
+  <si>
+    <t>320018686780</t>
+  </si>
+  <si>
+    <t>320018686806</t>
+  </si>
+  <si>
+    <t>320018686840</t>
+  </si>
+  <si>
+    <t>320018686861</t>
+  </si>
+  <si>
+    <t>320018686894</t>
+  </si>
+  <si>
+    <t>320018686910</t>
+  </si>
+  <si>
+    <t>320018686942</t>
+  </si>
+  <si>
+    <t>320018686964</t>
+  </si>
+  <si>
+    <t>320018687000</t>
+  </si>
+  <si>
+    <t>320018687022</t>
+  </si>
+  <si>
+    <t>320018687055</t>
+  </si>
+  <si>
+    <t>320018687077</t>
+  </si>
+  <si>
+    <t>320018687103</t>
+  </si>
+  <si>
+    <t>320018690202</t>
+  </si>
+  <si>
+    <t>320018690213</t>
+  </si>
+  <si>
+    <t>320018690246</t>
+  </si>
+  <si>
+    <t>320018690268</t>
+  </si>
+  <si>
+    <t>320018690305</t>
+  </si>
+  <si>
+    <t>320018690327</t>
+  </si>
+  <si>
+    <t>320018690350</t>
+  </si>
+  <si>
+    <t>320018690371</t>
+  </si>
+  <si>
+    <t>320018690408</t>
+  </si>
+  <si>
+    <t>320018690420</t>
+  </si>
+  <si>
+    <t>320018690463</t>
+  </si>
+  <si>
+    <t>320018690485</t>
+  </si>
+  <si>
+    <t>320018690511</t>
+  </si>
+  <si>
+    <t>320018690533</t>
+  </si>
+  <si>
+    <t>320018690566</t>
+  </si>
+  <si>
+    <t>320018690588</t>
+  </si>
+  <si>
+    <t>320018690625</t>
+  </si>
+  <si>
+    <t>320018690647</t>
+  </si>
+  <si>
+    <t>320018690670</t>
+  </si>
+  <si>
+    <t>320018690691</t>
+  </si>
+  <si>
+    <t>320018690728</t>
+  </si>
+  <si>
+    <t>320018703526</t>
+  </si>
+  <si>
+    <t>320018703537</t>
+  </si>
+  <si>
+    <t>320018703560</t>
+  </si>
+  <si>
+    <t>320018703581</t>
+  </si>
+  <si>
+    <t>320018703629</t>
+  </si>
+  <si>
+    <t>320018703640</t>
+  </si>
+  <si>
+    <t>320018703673</t>
+  </si>
+  <si>
+    <t>320018703695</t>
+  </si>
+  <si>
+    <t>320018703721</t>
+  </si>
+  <si>
+    <t>320018703743</t>
+  </si>
+  <si>
+    <t>320018703787</t>
+  </si>
+  <si>
+    <t>320018703802</t>
+  </si>
+  <si>
+    <t>320018703835</t>
+  </si>
+  <si>
+    <t>320018703857</t>
+  </si>
+  <si>
+    <t>320018703880</t>
+  </si>
+  <si>
+    <t>320018703905</t>
+  </si>
+  <si>
+    <t>320018703949</t>
+  </si>
+  <si>
+    <t>320018703960</t>
+  </si>
+  <si>
+    <t>320018703993</t>
+  </si>
+  <si>
+    <t>320018704018</t>
+  </si>
+  <si>
+    <t>320018704040</t>
+  </si>
+  <si>
+    <t>320018727924</t>
+  </si>
+  <si>
+    <t>320018727935</t>
+  </si>
+  <si>
+    <t>320018727968</t>
+  </si>
+  <si>
+    <t>320018727980</t>
+  </si>
+  <si>
+    <t>320018728026</t>
+  </si>
+  <si>
+    <t>320018728048</t>
+  </si>
+  <si>
+    <t>320018728070</t>
+  </si>
+  <si>
+    <t>320018728092</t>
+  </si>
+  <si>
+    <t>320018728129</t>
+  </si>
+  <si>
+    <t>320018728140</t>
+  </si>
+  <si>
+    <t>320018728184</t>
+  </si>
+  <si>
+    <t>320018728200</t>
+  </si>
+  <si>
+    <t>320018728232</t>
+  </si>
+  <si>
+    <t>320018728254</t>
+  </si>
+  <si>
+    <t>320018728287</t>
+  </si>
+  <si>
+    <t>320018728302</t>
+  </si>
+  <si>
+    <t>320018728346</t>
+  </si>
+  <si>
+    <t>320018728368</t>
+  </si>
+  <si>
+    <t>320018728390</t>
+  </si>
+  <si>
+    <t>320018728427</t>
+  </si>
+  <si>
+    <t>320018728450</t>
+  </si>
+  <si>
+    <t>320018735874</t>
+  </si>
+  <si>
+    <t>320018735885</t>
+  </si>
+  <si>
+    <t>320018735911</t>
+  </si>
+  <si>
+    <t>320018735933</t>
+  </si>
+  <si>
+    <t>320018735977</t>
+  </si>
+  <si>
+    <t>320018735999</t>
+  </si>
+  <si>
+    <t>320018736024</t>
+  </si>
+  <si>
+    <t>320018736046</t>
+  </si>
+  <si>
+    <t>320018736079</t>
+  </si>
+  <si>
+    <t>320018736090</t>
+  </si>
+  <si>
+    <t>320018736138</t>
+  </si>
+  <si>
+    <t>320018736150</t>
+  </si>
+  <si>
+    <t>320018736182</t>
+  </si>
+  <si>
+    <t>320018736208</t>
+  </si>
+  <si>
+    <t>320018736230</t>
+  </si>
+  <si>
+    <t>320018736252</t>
+  </si>
+  <si>
+    <t>320018736296</t>
+  </si>
+  <si>
+    <t>320018736311</t>
+  </si>
+  <si>
+    <t>320018736344</t>
+  </si>
+  <si>
+    <t>320018736366</t>
+  </si>
+  <si>
+    <t>320018736399</t>
+  </si>
+  <si>
+    <t>320018736470</t>
+  </si>
+  <si>
+    <t>320018736480</t>
+  </si>
+  <si>
+    <t>320018736517</t>
+  </si>
+  <si>
+    <t>320018736539</t>
+  </si>
+  <si>
+    <t>320018736572</t>
+  </si>
+  <si>
+    <t>320018736594</t>
+  </si>
+  <si>
+    <t>320018738910</t>
+  </si>
+  <si>
+    <t>320018738921</t>
+  </si>
+  <si>
+    <t>320018738954</t>
+  </si>
+  <si>
+    <t>320018738976</t>
+  </si>
+  <si>
+    <t>320018739012</t>
+  </si>
+  <si>
+    <t>320018739034</t>
+  </si>
+  <si>
+    <t>320018739067</t>
+  </si>
+  <si>
+    <t>320018739089</t>
+  </si>
+  <si>
+    <t>320018739310</t>
+  </si>
+  <si>
+    <t>320018739332</t>
+  </si>
+  <si>
+    <t>320018739376</t>
+  </si>
+  <si>
+    <t>320018739398</t>
+  </si>
+  <si>
+    <t>320018739424</t>
+  </si>
+  <si>
+    <t>320018739446</t>
+  </si>
+  <si>
+    <t>320018739479</t>
+  </si>
+  <si>
+    <t>320018739490</t>
+  </si>
+  <si>
+    <t>320018739538</t>
+  </si>
+  <si>
+    <t>320018739560</t>
+  </si>
+  <si>
+    <t>320018739593</t>
+  </si>
+  <si>
+    <t>320018739619</t>
+  </si>
+  <si>
+    <t>320018739641</t>
+  </si>
+  <si>
+    <t>320018744077</t>
+  </si>
+  <si>
+    <t>320018744088</t>
+  </si>
+  <si>
+    <t>320018744114</t>
+  </si>
+  <si>
+    <t>320018744136</t>
+  </si>
+  <si>
+    <t>320018744170</t>
+  </si>
+  <si>
+    <t>320018744191</t>
+  </si>
+  <si>
+    <t>320018744228</t>
+  </si>
+  <si>
+    <t>320018744240</t>
+  </si>
+  <si>
+    <t>320018744272</t>
+  </si>
+  <si>
+    <t>320018744294</t>
+  </si>
+  <si>
+    <t>320018744331</t>
+  </si>
+  <si>
+    <t>320018744353</t>
+  </si>
+  <si>
+    <t>320018744386</t>
+  </si>
+  <si>
+    <t>320018744401</t>
+  </si>
+  <si>
+    <t>320018744434</t>
+  </si>
+  <si>
+    <t>320018744456</t>
+  </si>
+  <si>
+    <t>320018744490</t>
+  </si>
+  <si>
+    <t>320018744515</t>
+  </si>
+  <si>
+    <t>320018744548</t>
+  </si>
+  <si>
+    <t>320018744560</t>
+  </si>
+  <si>
+    <t>320018744592</t>
+  </si>
+  <si>
+    <t>320018753715</t>
+  </si>
+  <si>
+    <t>320018753726</t>
+  </si>
+  <si>
+    <t>320018753759</t>
+  </si>
+  <si>
+    <t>320018753770</t>
+  </si>
+  <si>
+    <t>320018753818</t>
+  </si>
+  <si>
+    <t>320018753840</t>
+  </si>
+  <si>
+    <t>320018753884</t>
+  </si>
+  <si>
+    <t>320018753900</t>
+  </si>
+  <si>
+    <t>320018753932</t>
+  </si>
+  <si>
+    <t>320018753954</t>
+  </si>
+  <si>
+    <t>320018753998</t>
+  </si>
+  <si>
+    <t>320018754012</t>
+  </si>
+  <si>
+    <t>320018754045</t>
+  </si>
+  <si>
+    <t>320018754067</t>
+  </si>
+  <si>
+    <t>320018754090</t>
+  </si>
+  <si>
+    <t>320018754115</t>
+  </si>
+  <si>
+    <t>320018754159</t>
+  </si>
+  <si>
+    <t>320018754170</t>
+  </si>
+  <si>
+    <t>320018754207</t>
+  </si>
+  <si>
+    <t>320018754230</t>
+  </si>
+  <si>
+    <t>320018754262</t>
+  </si>
+  <si>
+    <t>320018763304</t>
+  </si>
+  <si>
+    <t>320018763315</t>
+  </si>
+  <si>
+    <t>320018763348</t>
+  </si>
+  <si>
+    <t>320018763360</t>
+  </si>
+  <si>
+    <t>320018763407</t>
+  </si>
+  <si>
+    <t>320018763429</t>
+  </si>
+  <si>
+    <t>320018763451</t>
+  </si>
+  <si>
+    <t>320018763473</t>
+  </si>
+  <si>
+    <t>320018763500</t>
+  </si>
+  <si>
+    <t>320018763521</t>
+  </si>
+  <si>
+    <t>320018763565</t>
+  </si>
+  <si>
+    <t>320018763587</t>
+  </si>
+  <si>
+    <t>320018763613</t>
+  </si>
+  <si>
+    <t>320018763635</t>
+  </si>
+  <si>
+    <t>320018763668</t>
+  </si>
+  <si>
+    <t>320018763680</t>
+  </si>
+  <si>
+    <t>320018763727</t>
+  </si>
+  <si>
+    <t>320018763749</t>
+  </si>
+  <si>
+    <t>320018763771</t>
+  </si>
+  <si>
+    <t>320018763793</t>
+  </si>
+  <si>
+    <t>320018763820</t>
+  </si>
+  <si>
+    <t>320018763874</t>
+  </si>
+  <si>
+    <t>320018763885</t>
+  </si>
+  <si>
+    <t>320018763911</t>
+  </si>
+  <si>
+    <t>320018763933</t>
+  </si>
+  <si>
+    <t>320018763977</t>
+  </si>
+  <si>
+    <t>320018763999</t>
+  </si>
+  <si>
+    <t>320018764024</t>
+  </si>
+  <si>
+    <t>320018764046</t>
+  </si>
+  <si>
+    <t>320018764079</t>
+  </si>
+  <si>
+    <t>320018764090</t>
+  </si>
+  <si>
+    <t>320018764138</t>
+  </si>
+  <si>
+    <t>320018764150</t>
+  </si>
+  <si>
+    <t>320018764182</t>
+  </si>
+  <si>
+    <t>320018764208</t>
+  </si>
+  <si>
+    <t>320018764230</t>
+  </si>
+  <si>
+    <t>320018764252</t>
+  </si>
+  <si>
+    <t>320018764296</t>
+  </si>
+  <si>
+    <t>320018764311</t>
+  </si>
+  <si>
+    <t>320018764344</t>
+  </si>
+  <si>
+    <t>320018764366</t>
+  </si>
+  <si>
+    <t>320018764399</t>
+  </si>
+  <si>
+    <t>320018787735</t>
+  </si>
+  <si>
+    <t>320018787746</t>
+  </si>
+  <si>
+    <t>320018787779</t>
+  </si>
+  <si>
+    <t>320018787790</t>
+  </si>
+  <si>
+    <t>320018787838</t>
+  </si>
+  <si>
+    <t>320018787893</t>
+  </si>
+  <si>
+    <t>320018787908</t>
+  </si>
+  <si>
+    <t>320018787930</t>
+  </si>
+  <si>
+    <t>320018787952</t>
+  </si>
+  <si>
+    <t>320018787996</t>
+  </si>
+  <si>
+    <t>320018788514</t>
+  </si>
+  <si>
+    <t>320018792274</t>
+  </si>
+  <si>
+    <t>320018792300</t>
+  </si>
+  <si>
+    <t>320018792322</t>
+  </si>
+  <si>
+    <t>320018792366</t>
+  </si>
+  <si>
+    <t>320018792388</t>
+  </si>
+  <si>
+    <t>320018792414</t>
+  </si>
+  <si>
+    <t>320018792436</t>
+  </si>
+  <si>
+    <t>320018792469</t>
+  </si>
+  <si>
+    <t>320018792480</t>
+  </si>
+  <si>
+    <t>320018792528</t>
+  </si>
+  <si>
+    <t>320018792540</t>
+  </si>
+  <si>
+    <t>320018792572</t>
+  </si>
+  <si>
+    <t>320018792594</t>
+  </si>
+  <si>
+    <t>320018792620</t>
+  </si>
+  <si>
+    <t>320018792642</t>
+  </si>
+  <si>
+    <t>320018792686</t>
+  </si>
+  <si>
+    <t>320018792701</t>
+  </si>
+  <si>
+    <t>320018792734</t>
+  </si>
+  <si>
+    <t>320018792756</t>
+  </si>
+  <si>
+    <t>320018792789</t>
+  </si>
+  <si>
+    <t>320018799382</t>
+  </si>
+  <si>
+    <t>320018799393</t>
+  </si>
+  <si>
+    <t>320018799420</t>
+  </si>
+  <si>
+    <t>320018799441</t>
+  </si>
+  <si>
+    <t>320018799485</t>
+  </si>
+  <si>
+    <t>320018799500</t>
+  </si>
+  <si>
+    <t>320018799533</t>
+  </si>
+  <si>
+    <t>320018799625</t>
+  </si>
+  <si>
+    <t>320018799658</t>
+  </si>
+  <si>
+    <t>320018799670</t>
+  </si>
+  <si>
+    <t>320018799717</t>
+  </si>
+  <si>
+    <t>320018799739</t>
+  </si>
+  <si>
+    <t>320018799761</t>
+  </si>
+  <si>
+    <t>320018799783</t>
+  </si>
+  <si>
+    <t>320018799810</t>
+  </si>
+  <si>
+    <t>320018799831</t>
+  </si>
+  <si>
+    <t>320018799875</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +3071,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>385</v>
+        <v>810</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1858,7 +3121,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>386</v>
+        <v>811</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -1900,7 +3163,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>387</v>
+        <v>812</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -1952,10 +3215,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>388</v>
+        <v>813</v>
       </c>
       <c r="D5" t="s">
-        <v>388</v>
+        <v>813</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2006,10 +3269,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>389</v>
+        <v>814</v>
       </c>
       <c r="D6" t="s">
-        <v>389</v>
+        <v>814</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -2064,10 +3327,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>390</v>
+        <v>815</v>
       </c>
       <c r="D7" t="s">
-        <v>390</v>
+        <v>815</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -2128,7 +3391,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>391</v>
+        <v>816</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -2184,7 +3447,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>392</v>
+        <v>817</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -2224,7 +3487,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>393</v>
+        <v>818</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -2264,7 +3527,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>819</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -2304,7 +3567,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>395</v>
+        <v>820</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -2346,10 +3609,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>396</v>
+        <v>821</v>
       </c>
       <c r="D13" t="s">
-        <v>396</v>
+        <v>821</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2400,10 +3663,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>397</v>
+        <v>822</v>
       </c>
       <c r="D14" t="s">
-        <v>397</v>
+        <v>822</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2454,10 +3717,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>398</v>
+        <v>823</v>
       </c>
       <c r="D15" t="s">
-        <v>398</v>
+        <v>823</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2508,10 +3771,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>399</v>
+        <v>824</v>
       </c>
       <c r="D16" t="s">
-        <v>399</v>
+        <v>824</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2562,10 +3825,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>400</v>
+        <v>825</v>
       </c>
       <c r="D17" t="s">
-        <v>400</v>
+        <v>825</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2616,7 +3879,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>401</v>
+        <v>826</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -2658,7 +3921,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>402</v>
+        <v>806</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -2710,7 +3973,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>403</v>
+        <v>807</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -2762,7 +4025,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>404</v>
+        <v>808</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -2816,7 +4079,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>405</v>
+        <v>809</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 15th june 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4449" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4554" uniqueCount="848">
   <si>
     <t>Sno</t>
   </si>
@@ -2495,6 +2495,69 @@
   </si>
   <si>
     <t>320018799875</t>
+  </si>
+  <si>
+    <t>320018813081</t>
+  </si>
+  <si>
+    <t>320018813092</t>
+  </si>
+  <si>
+    <t>320018813129</t>
+  </si>
+  <si>
+    <t>320018813140</t>
+  </si>
+  <si>
+    <t>320018813184</t>
+  </si>
+  <si>
+    <t>320018813200</t>
+  </si>
+  <si>
+    <t>320018813232</t>
+  </si>
+  <si>
+    <t>320018813254</t>
+  </si>
+  <si>
+    <t>320018813287</t>
+  </si>
+  <si>
+    <t>320018813302</t>
+  </si>
+  <si>
+    <t>320018813346</t>
+  </si>
+  <si>
+    <t>320018813449</t>
+  </si>
+  <si>
+    <t>320018813471</t>
+  </si>
+  <si>
+    <t>320018813493</t>
+  </si>
+  <si>
+    <t>320018813520</t>
+  </si>
+  <si>
+    <t>320018813541</t>
+  </si>
+  <si>
+    <t>320018813585</t>
+  </si>
+  <si>
+    <t>320018813600</t>
+  </si>
+  <si>
+    <t>320018813850</t>
+  </si>
+  <si>
+    <t>320018813872</t>
+  </si>
+  <si>
+    <t>320018813909</t>
   </si>
 </sst>
 </file>
@@ -3071,7 +3134,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>810</v>
+        <v>827</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3121,7 +3184,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>811</v>
+        <v>828</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3163,7 +3226,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>812</v>
+        <v>829</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -3215,10 +3278,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>813</v>
+        <v>830</v>
       </c>
       <c r="D5" t="s">
-        <v>813</v>
+        <v>830</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3269,10 +3332,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>814</v>
+        <v>831</v>
       </c>
       <c r="D6" t="s">
-        <v>814</v>
+        <v>831</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -3327,10 +3390,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>815</v>
+        <v>832</v>
       </c>
       <c r="D7" t="s">
-        <v>815</v>
+        <v>832</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -3391,7 +3454,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>816</v>
+        <v>833</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -3447,7 +3510,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>817</v>
+        <v>834</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -3487,7 +3550,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>818</v>
+        <v>835</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -3527,7 +3590,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>819</v>
+        <v>836</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -3567,7 +3630,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>820</v>
+        <v>837</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -3609,10 +3672,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>821</v>
+        <v>838</v>
       </c>
       <c r="D13" t="s">
-        <v>821</v>
+        <v>838</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -3663,10 +3726,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>822</v>
+        <v>839</v>
       </c>
       <c r="D14" t="s">
-        <v>822</v>
+        <v>839</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -3717,10 +3780,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>823</v>
+        <v>840</v>
       </c>
       <c r="D15" t="s">
-        <v>823</v>
+        <v>840</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -3771,10 +3834,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>824</v>
+        <v>841</v>
       </c>
       <c r="D16" t="s">
-        <v>824</v>
+        <v>841</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -3825,10 +3888,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>825</v>
+        <v>842</v>
       </c>
       <c r="D17" t="s">
-        <v>825</v>
+        <v>842</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -3879,7 +3942,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>826</v>
+        <v>843</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -3921,7 +3984,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>806</v>
+        <v>844</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -3973,7 +4036,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>807</v>
+        <v>845</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4025,7 +4088,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>808</v>
+        <v>846</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4079,7 +4142,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>809</v>
+        <v>847</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
changes of 18th june 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4554" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4640" uniqueCount="912">
   <si>
     <t>Sno</t>
   </si>
@@ -2558,6 +2558,198 @@
   </si>
   <si>
     <t>320018813909</t>
+  </si>
+  <si>
+    <t>320018499958</t>
+  </si>
+  <si>
+    <t>320018499969</t>
+  </si>
+  <si>
+    <t>320018499991</t>
+  </si>
+  <si>
+    <t>320018500017</t>
+  </si>
+  <si>
+    <t>320018500050</t>
+  </si>
+  <si>
+    <t>320018500072</t>
+  </si>
+  <si>
+    <t>320018500109</t>
+  </si>
+  <si>
+    <t>320018500120</t>
+  </si>
+  <si>
+    <t>320018500830</t>
+  </si>
+  <si>
+    <t>320018500852</t>
+  </si>
+  <si>
+    <t>320018500896</t>
+  </si>
+  <si>
+    <t>320018500911</t>
+  </si>
+  <si>
+    <t>320018500944</t>
+  </si>
+  <si>
+    <t>320018500966</t>
+  </si>
+  <si>
+    <t>320018500999</t>
+  </si>
+  <si>
+    <t>320018501035</t>
+  </si>
+  <si>
+    <t>320018501079</t>
+  </si>
+  <si>
+    <t>320018501090</t>
+  </si>
+  <si>
+    <t>320018501127</t>
+  </si>
+  <si>
+    <t>320018501149</t>
+  </si>
+  <si>
+    <t>320018501171</t>
+  </si>
+  <si>
+    <t>320018502833</t>
+  </si>
+  <si>
+    <t>320018502844</t>
+  </si>
+  <si>
+    <t>320018502888</t>
+  </si>
+  <si>
+    <t>320018502903</t>
+  </si>
+  <si>
+    <t>320018502947</t>
+  </si>
+  <si>
+    <t>320018502969</t>
+  </si>
+  <si>
+    <t>320018503005</t>
+  </si>
+  <si>
+    <t>320018503027</t>
+  </si>
+  <si>
+    <t>320018503050</t>
+  </si>
+  <si>
+    <t>320018503071</t>
+  </si>
+  <si>
+    <t>320018503119</t>
+  </si>
+  <si>
+    <t>320018503130</t>
+  </si>
+  <si>
+    <t>320018503163</t>
+  </si>
+  <si>
+    <t>320018503185</t>
+  </si>
+  <si>
+    <t>320018503211</t>
+  </si>
+  <si>
+    <t>320018503244</t>
+  </si>
+  <si>
+    <t>320018503288</t>
+  </si>
+  <si>
+    <t>320018503303</t>
+  </si>
+  <si>
+    <t>320018503336</t>
+  </si>
+  <si>
+    <t>320018503358</t>
+  </si>
+  <si>
+    <t>320018503380</t>
+  </si>
+  <si>
+    <t>320018505660</t>
+  </si>
+  <si>
+    <t>320018505670</t>
+  </si>
+  <si>
+    <t>320018505707</t>
+  </si>
+  <si>
+    <t>320018505729</t>
+  </si>
+  <si>
+    <t>320018505762</t>
+  </si>
+  <si>
+    <t>320018505784</t>
+  </si>
+  <si>
+    <t>320018505810</t>
+  </si>
+  <si>
+    <t>320018505832</t>
+  </si>
+  <si>
+    <t>320018505865</t>
+  </si>
+  <si>
+    <t>320018505887</t>
+  </si>
+  <si>
+    <t>320018505924</t>
+  </si>
+  <si>
+    <t>320018511882</t>
+  </si>
+  <si>
+    <t>320018511996</t>
+  </si>
+  <si>
+    <t>320018512021</t>
+  </si>
+  <si>
+    <t>320018512098</t>
+  </si>
+  <si>
+    <t>320018512135</t>
+  </si>
+  <si>
+    <t>320018512205</t>
+  </si>
+  <si>
+    <t>320018512238</t>
+  </si>
+  <si>
+    <t>320018512250</t>
+  </si>
+  <si>
+    <t>320018512282</t>
+  </si>
+  <si>
+    <t>320018512319</t>
+  </si>
+  <si>
+    <t>320018512400</t>
   </si>
 </sst>
 </file>
@@ -3000,7 +3192,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD24"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -3134,7 +3326,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>827</v>
+        <v>901</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3184,7 +3376,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>828</v>
+        <v>902</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3226,7 +3418,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>829</v>
+        <v>903</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -3278,10 +3470,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>830</v>
+        <v>904</v>
       </c>
       <c r="D5" t="s">
-        <v>830</v>
+        <v>904</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3332,10 +3524,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>831</v>
+        <v>905</v>
       </c>
       <c r="D6" t="s">
-        <v>831</v>
+        <v>905</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -3390,10 +3582,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>832</v>
+        <v>906</v>
       </c>
       <c r="D7" t="s">
-        <v>832</v>
+        <v>906</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -3454,7 +3646,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>833</v>
+        <v>907</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -3510,7 +3702,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>834</v>
+        <v>908</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -3550,7 +3742,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>835</v>
+        <v>909</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -3590,7 +3782,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>836</v>
+        <v>910</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -3630,7 +3822,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>837</v>
+        <v>911</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -3672,10 +3864,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>838</v>
+        <v>880</v>
       </c>
       <c r="D13" t="s">
-        <v>838</v>
+        <v>880</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -3726,10 +3918,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>839</v>
+        <v>881</v>
       </c>
       <c r="D14" t="s">
-        <v>839</v>
+        <v>881</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -3780,10 +3972,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>840</v>
+        <v>882</v>
       </c>
       <c r="D15" t="s">
-        <v>840</v>
+        <v>882</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -3834,10 +4026,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>841</v>
+        <v>883</v>
       </c>
       <c r="D16" t="s">
-        <v>841</v>
+        <v>883</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -3888,10 +4080,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>842</v>
+        <v>884</v>
       </c>
       <c r="D17" t="s">
-        <v>842</v>
+        <v>884</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -3942,7 +4134,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>843</v>
+        <v>885</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -3984,7 +4176,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>844</v>
+        <v>886</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4036,7 +4228,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>845</v>
+        <v>887</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4088,7 +4280,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>846</v>
+        <v>888</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4142,7 +4334,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>847</v>
+        <v>889</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 21st June 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4640" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4796" uniqueCount="933">
   <si>
     <t>Sno</t>
   </si>
@@ -2750,6 +2750,69 @@
   </si>
   <si>
     <t>320018512400</t>
+  </si>
+  <si>
+    <t>320018538422</t>
+  </si>
+  <si>
+    <t>320018538433</t>
+  </si>
+  <si>
+    <t>320018538466</t>
+  </si>
+  <si>
+    <t>320018538488</t>
+  </si>
+  <si>
+    <t>320018538525</t>
+  </si>
+  <si>
+    <t>320018538547</t>
+  </si>
+  <si>
+    <t>320018538570</t>
+  </si>
+  <si>
+    <t>320018538591</t>
+  </si>
+  <si>
+    <t>320018538628</t>
+  </si>
+  <si>
+    <t>320018538640</t>
+  </si>
+  <si>
+    <t>320018538694</t>
+  </si>
+  <si>
+    <t>320018538710</t>
+  </si>
+  <si>
+    <t>320018538742</t>
+  </si>
+  <si>
+    <t>320018538775</t>
+  </si>
+  <si>
+    <t>320018538801</t>
+  </si>
+  <si>
+    <t>320018538823</t>
+  </si>
+  <si>
+    <t>320018538867</t>
+  </si>
+  <si>
+    <t>320018538889</t>
+  </si>
+  <si>
+    <t>320018538915</t>
+  </si>
+  <si>
+    <t>320018538937</t>
+  </si>
+  <si>
+    <t>320018538960</t>
   </si>
 </sst>
 </file>
@@ -3326,7 +3389,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>901</v>
+        <v>912</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3376,7 +3439,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>902</v>
+        <v>913</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3394,7 +3457,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -3418,7 +3481,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>903</v>
+        <v>914</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -3470,10 +3533,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>904</v>
+        <v>915</v>
       </c>
       <c r="D5" t="s">
-        <v>904</v>
+        <v>915</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3524,10 +3587,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>905</v>
+        <v>916</v>
       </c>
       <c r="D6" t="s">
-        <v>905</v>
+        <v>916</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -3582,10 +3645,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>906</v>
+        <v>917</v>
       </c>
       <c r="D7" t="s">
-        <v>906</v>
+        <v>917</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -3646,7 +3709,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>907</v>
+        <v>918</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -3702,7 +3765,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>908</v>
+        <v>919</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -3742,7 +3805,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>909</v>
+        <v>920</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -3782,7 +3845,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>910</v>
+        <v>921</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -3822,7 +3885,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>911</v>
+        <v>922</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -3864,10 +3927,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>880</v>
+        <v>923</v>
       </c>
       <c r="D13" t="s">
-        <v>880</v>
+        <v>923</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -3918,10 +3981,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>881</v>
+        <v>924</v>
       </c>
       <c r="D14" t="s">
-        <v>881</v>
+        <v>924</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -3972,10 +4035,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>882</v>
+        <v>925</v>
       </c>
       <c r="D15" t="s">
-        <v>882</v>
+        <v>925</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -4026,10 +4089,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>883</v>
+        <v>926</v>
       </c>
       <c r="D16" t="s">
-        <v>883</v>
+        <v>926</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -4080,10 +4143,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>884</v>
+        <v>927</v>
       </c>
       <c r="D17" t="s">
-        <v>884</v>
+        <v>927</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -4134,7 +4197,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>885</v>
+        <v>928</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -4176,7 +4239,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>886</v>
+        <v>929</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4228,7 +4291,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>887</v>
+        <v>930</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4280,7 +4343,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>888</v>
+        <v>931</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4334,7 +4397,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>889</v>
+        <v>932</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes in login script
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4796" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5112" uniqueCount="997">
   <si>
     <t>Sno</t>
   </si>
@@ -2813,6 +2813,198 @@
   </si>
   <si>
     <t>320018538960</t>
+  </si>
+  <si>
+    <t>320018539874</t>
+  </si>
+  <si>
+    <t>320018540010</t>
+  </si>
+  <si>
+    <t>320018540021</t>
+  </si>
+  <si>
+    <t>320018540054</t>
+  </si>
+  <si>
+    <t>320018540098</t>
+  </si>
+  <si>
+    <t>320018540135</t>
+  </si>
+  <si>
+    <t>320018540157</t>
+  </si>
+  <si>
+    <t>320018540180</t>
+  </si>
+  <si>
+    <t>320018540205</t>
+  </si>
+  <si>
+    <t>320018540238</t>
+  </si>
+  <si>
+    <t>320018540271</t>
+  </si>
+  <si>
+    <t>320018540320</t>
+  </si>
+  <si>
+    <t>320018540363</t>
+  </si>
+  <si>
+    <t>320018540396</t>
+  </si>
+  <si>
+    <t>320018540411</t>
+  </si>
+  <si>
+    <t>320018540444</t>
+  </si>
+  <si>
+    <t>320018540466</t>
+  </si>
+  <si>
+    <t>320018540514</t>
+  </si>
+  <si>
+    <t>320018540547</t>
+  </si>
+  <si>
+    <t>320018540570</t>
+  </si>
+  <si>
+    <t>320018540606</t>
+  </si>
+  <si>
+    <t>320018540639</t>
+  </si>
+  <si>
+    <t>320018541289</t>
+  </si>
+  <si>
+    <t>320018541290</t>
+  </si>
+  <si>
+    <t>320018541326</t>
+  </si>
+  <si>
+    <t>320018541348</t>
+  </si>
+  <si>
+    <t>320018541381</t>
+  </si>
+  <si>
+    <t>320018541407</t>
+  </si>
+  <si>
+    <t>320018541430</t>
+  </si>
+  <si>
+    <t>320018541451</t>
+  </si>
+  <si>
+    <t>320018541484</t>
+  </si>
+  <si>
+    <t>320018541500</t>
+  </si>
+  <si>
+    <t>320018541543</t>
+  </si>
+  <si>
+    <t>320018541565</t>
+  </si>
+  <si>
+    <t>320018541598</t>
+  </si>
+  <si>
+    <t>320018541613</t>
+  </si>
+  <si>
+    <t>320018541646</t>
+  </si>
+  <si>
+    <t>320018541668</t>
+  </si>
+  <si>
+    <t>320018541705</t>
+  </si>
+  <si>
+    <t>320018541727</t>
+  </si>
+  <si>
+    <t>320018541750</t>
+  </si>
+  <si>
+    <t>320018541771</t>
+  </si>
+  <si>
+    <t>320018541808</t>
+  </si>
+  <si>
+    <t>320018543178</t>
+  </si>
+  <si>
+    <t>320018543226</t>
+  </si>
+  <si>
+    <t>320018543259</t>
+  </si>
+  <si>
+    <t>320018543270</t>
+  </si>
+  <si>
+    <t>320018543318</t>
+  </si>
+  <si>
+    <t>320018543330</t>
+  </si>
+  <si>
+    <t>320018543362</t>
+  </si>
+  <si>
+    <t>320018543384</t>
+  </si>
+  <si>
+    <t>320018543410</t>
+  </si>
+  <si>
+    <t>320018543432</t>
+  </si>
+  <si>
+    <t>320018543476</t>
+  </si>
+  <si>
+    <t>320018543498</t>
+  </si>
+  <si>
+    <t>320018543524</t>
+  </si>
+  <si>
+    <t>320018543546</t>
+  </si>
+  <si>
+    <t>320018543579</t>
+  </si>
+  <si>
+    <t>320018548011</t>
+  </si>
+  <si>
+    <t>320018548055</t>
+  </si>
+  <si>
+    <t>320018548077</t>
+  </si>
+  <si>
+    <t>320018548103</t>
+  </si>
+  <si>
+    <t>320018548125</t>
+  </si>
+  <si>
+    <t>320018548158</t>
   </si>
 </sst>
 </file>
@@ -3255,7 +3447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -3389,7 +3581,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>912</v>
+        <v>976</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3439,7 +3631,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>913</v>
+        <v>977</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3457,7 +3649,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -3481,7 +3673,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>914</v>
+        <v>978</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -3533,10 +3725,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>915</v>
+        <v>979</v>
       </c>
       <c r="D5" t="s">
-        <v>915</v>
+        <v>979</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3587,10 +3779,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>916</v>
+        <v>980</v>
       </c>
       <c r="D6" t="s">
-        <v>916</v>
+        <v>980</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -3645,10 +3837,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>917</v>
+        <v>981</v>
       </c>
       <c r="D7" t="s">
-        <v>917</v>
+        <v>981</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -3709,7 +3901,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>918</v>
+        <v>982</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -3765,7 +3957,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>919</v>
+        <v>983</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -3805,7 +3997,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>920</v>
+        <v>984</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -3845,7 +4037,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>921</v>
+        <v>985</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -3885,7 +4077,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>922</v>
+        <v>986</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -3927,10 +4119,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>923</v>
+        <v>987</v>
       </c>
       <c r="D13" t="s">
-        <v>923</v>
+        <v>987</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -3981,10 +4173,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>924</v>
+        <v>988</v>
       </c>
       <c r="D14" t="s">
-        <v>924</v>
+        <v>988</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -4035,10 +4227,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>925</v>
+        <v>989</v>
       </c>
       <c r="D15" t="s">
-        <v>925</v>
+        <v>989</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -4089,10 +4281,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>926</v>
+        <v>990</v>
       </c>
       <c r="D16" t="s">
-        <v>926</v>
+        <v>990</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -4143,10 +4335,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>927</v>
+        <v>991</v>
       </c>
       <c r="D17" t="s">
-        <v>927</v>
+        <v>991</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -4197,7 +4389,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>928</v>
+        <v>992</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -4239,7 +4431,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>929</v>
+        <v>993</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4291,7 +4483,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>930</v>
+        <v>994</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4343,7 +4535,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>931</v>
+        <v>995</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4397,7 +4589,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>932</v>
+        <v>996</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of New Pre-Prod URL
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5112" uniqueCount="997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5322" uniqueCount="1039">
   <si>
     <t>Sno</t>
   </si>
@@ -3005,6 +3005,132 @@
   </si>
   <si>
     <t>320018548158</t>
+  </si>
+  <si>
+    <t>320018568517</t>
+  </si>
+  <si>
+    <t>320018568528</t>
+  </si>
+  <si>
+    <t>320018568550</t>
+  </si>
+  <si>
+    <t>320018568572</t>
+  </si>
+  <si>
+    <t>320018568610</t>
+  </si>
+  <si>
+    <t>320018568631</t>
+  </si>
+  <si>
+    <t>320018568664</t>
+  </si>
+  <si>
+    <t>320018568686</t>
+  </si>
+  <si>
+    <t>320018568712</t>
+  </si>
+  <si>
+    <t>320018568734</t>
+  </si>
+  <si>
+    <t>320018568778</t>
+  </si>
+  <si>
+    <t>320018568790</t>
+  </si>
+  <si>
+    <t>320018568826</t>
+  </si>
+  <si>
+    <t>320018568848</t>
+  </si>
+  <si>
+    <t>320018568870</t>
+  </si>
+  <si>
+    <t>320018568892</t>
+  </si>
+  <si>
+    <t>320018568930</t>
+  </si>
+  <si>
+    <t>320018568951</t>
+  </si>
+  <si>
+    <t>320018568984</t>
+  </si>
+  <si>
+    <t>320018569009</t>
+  </si>
+  <si>
+    <t>320018569031</t>
+  </si>
+  <si>
+    <t>320018589548</t>
+  </si>
+  <si>
+    <t>320018589559</t>
+  </si>
+  <si>
+    <t>320018589581</t>
+  </si>
+  <si>
+    <t>320018589607</t>
+  </si>
+  <si>
+    <t>320018589640</t>
+  </si>
+  <si>
+    <t>320018589662</t>
+  </si>
+  <si>
+    <t>320018589695</t>
+  </si>
+  <si>
+    <t>320018589710</t>
+  </si>
+  <si>
+    <t>320018589743</t>
+  </si>
+  <si>
+    <t>320018589765</t>
+  </si>
+  <si>
+    <t>320018589802</t>
+  </si>
+  <si>
+    <t>320018589824</t>
+  </si>
+  <si>
+    <t>320018589857</t>
+  </si>
+  <si>
+    <t>320018589879</t>
+  </si>
+  <si>
+    <t>320018589905</t>
+  </si>
+  <si>
+    <t>320018589927</t>
+  </si>
+  <si>
+    <t>320018589960</t>
+  </si>
+  <si>
+    <t>320018589982</t>
+  </si>
+  <si>
+    <t>320018590015</t>
+  </si>
+  <si>
+    <t>320018590037</t>
+  </si>
+  <si>
+    <t>320018590060</t>
   </si>
 </sst>
 </file>
@@ -3581,7 +3707,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>976</v>
+        <v>1018</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3631,7 +3757,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>977</v>
+        <v>1019</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3673,7 +3799,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>978</v>
+        <v>1020</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -3725,10 +3851,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>979</v>
+        <v>1021</v>
       </c>
       <c r="D5" t="s">
-        <v>979</v>
+        <v>1021</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3779,10 +3905,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>980</v>
+        <v>1022</v>
       </c>
       <c r="D6" t="s">
-        <v>980</v>
+        <v>1022</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -3837,10 +3963,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>981</v>
+        <v>1023</v>
       </c>
       <c r="D7" t="s">
-        <v>981</v>
+        <v>1023</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -3901,7 +4027,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>982</v>
+        <v>1024</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -3957,7 +4083,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>983</v>
+        <v>1025</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -3997,7 +4123,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>984</v>
+        <v>1026</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -4037,7 +4163,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>985</v>
+        <v>1027</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -4077,7 +4203,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>986</v>
+        <v>1028</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -4119,10 +4245,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>987</v>
+        <v>1029</v>
       </c>
       <c r="D13" t="s">
-        <v>987</v>
+        <v>1029</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -4173,10 +4299,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>988</v>
+        <v>1030</v>
       </c>
       <c r="D14" t="s">
-        <v>988</v>
+        <v>1030</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -4227,10 +4353,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>989</v>
+        <v>1031</v>
       </c>
       <c r="D15" t="s">
-        <v>989</v>
+        <v>1031</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -4281,10 +4407,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>990</v>
+        <v>1032</v>
       </c>
       <c r="D16" t="s">
-        <v>990</v>
+        <v>1032</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -4335,10 +4461,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>991</v>
+        <v>1033</v>
       </c>
       <c r="D17" t="s">
-        <v>991</v>
+        <v>1033</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -4389,7 +4515,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>992</v>
+        <v>1034</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -4431,7 +4557,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>993</v>
+        <v>1035</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4483,7 +4609,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>994</v>
+        <v>1036</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4535,7 +4661,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>995</v>
+        <v>1037</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4589,7 +4715,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>996</v>
+        <v>1038</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of webdriver exception
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/bin/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5322" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5427" uniqueCount="1060">
   <si>
     <t>Sno</t>
   </si>
@@ -3131,6 +3131,69 @@
   </si>
   <si>
     <t>320018590060</t>
+  </si>
+  <si>
+    <t>320018594180</t>
+  </si>
+  <si>
+    <t>320018594190</t>
+  </si>
+  <si>
+    <t>320018594227</t>
+  </si>
+  <si>
+    <t>320018594249</t>
+  </si>
+  <si>
+    <t>320018594282</t>
+  </si>
+  <si>
+    <t>320018594308</t>
+  </si>
+  <si>
+    <t>320018594330</t>
+  </si>
+  <si>
+    <t>320018594352</t>
+  </si>
+  <si>
+    <t>320018594385</t>
+  </si>
+  <si>
+    <t>320018594400</t>
+  </si>
+  <si>
+    <t>320018594444</t>
+  </si>
+  <si>
+    <t>320018594466</t>
+  </si>
+  <si>
+    <t>320018594499</t>
+  </si>
+  <si>
+    <t>320018594514</t>
+  </si>
+  <si>
+    <t>320018594547</t>
+  </si>
+  <si>
+    <t>320018594569</t>
+  </si>
+  <si>
+    <t>320018594606</t>
+  </si>
+  <si>
+    <t>320018594628</t>
+  </si>
+  <si>
+    <t>320018594650</t>
+  </si>
+  <si>
+    <t>320018594672</t>
+  </si>
+  <si>
+    <t>320018594709</t>
   </si>
 </sst>
 </file>
@@ -3707,7 +3770,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1018</v>
+        <v>1039</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3757,7 +3820,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1019</v>
+        <v>1040</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3799,7 +3862,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1020</v>
+        <v>1041</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -3851,10 +3914,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1021</v>
+        <v>1042</v>
       </c>
       <c r="D5" t="s">
-        <v>1021</v>
+        <v>1042</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3905,10 +3968,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1022</v>
+        <v>1043</v>
       </c>
       <c r="D6" t="s">
-        <v>1022</v>
+        <v>1043</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -3963,10 +4026,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1023</v>
+        <v>1044</v>
       </c>
       <c r="D7" t="s">
-        <v>1023</v>
+        <v>1044</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4027,7 +4090,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1024</v>
+        <v>1045</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -4083,7 +4146,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1025</v>
+        <v>1046</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -4123,7 +4186,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1026</v>
+        <v>1047</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -4163,7 +4226,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1027</v>
+        <v>1048</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -4203,7 +4266,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1028</v>
+        <v>1049</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -4245,10 +4308,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1029</v>
+        <v>1050</v>
       </c>
       <c r="D13" t="s">
-        <v>1029</v>
+        <v>1050</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -4299,10 +4362,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1030</v>
+        <v>1051</v>
       </c>
       <c r="D14" t="s">
-        <v>1030</v>
+        <v>1051</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -4353,10 +4416,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1031</v>
+        <v>1052</v>
       </c>
       <c r="D15" t="s">
-        <v>1031</v>
+        <v>1052</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -4407,10 +4470,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1032</v>
+        <v>1053</v>
       </c>
       <c r="D16" t="s">
-        <v>1032</v>
+        <v>1053</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -4461,10 +4524,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1033</v>
+        <v>1054</v>
       </c>
       <c r="D17" t="s">
-        <v>1033</v>
+        <v>1054</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -4515,7 +4578,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1034</v>
+        <v>1055</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -4557,7 +4620,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1035</v>
+        <v>1056</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4609,7 +4672,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1036</v>
+        <v>1057</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4661,7 +4724,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1037</v>
+        <v>1058</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4715,7 +4778,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1038</v>
+        <v>1059</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>